<commit_message>
Add all fine-tuning scripts
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="837" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87C403F8-D412-4EFD-91CA-D1979274D602}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -672,6 +672,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -693,12 +792,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,60 +804,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -777,6 +825,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -788,57 +839,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1165,13 +1165,13 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="60">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1197,9 +1197,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1223,9 +1223,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1242,9 +1242,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1261,9 +1261,9 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35">
+      <c r="A6" s="62"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1282,9 +1282,9 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1301,9 +1301,9 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1320,9 +1320,9 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1339,9 +1339,9 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35">
+      <c r="A10" s="62"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1360,9 +1360,9 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1379,9 +1379,9 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1398,9 +1398,9 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1423,9 +1423,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35">
+      <c r="A14" s="62"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1453,9 +1453,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1472,9 +1472,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1491,9 +1491,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1510,11 +1510,11 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
-      <c r="B18" s="25">
+      <c r="A18" s="62"/>
+      <c r="B18" s="58">
         <v>1</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1529,9 +1529,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1546,9 +1546,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="35"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1563,9 +1563,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="35"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1580,11 +1580,11 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35">
+      <c r="A22" s="62"/>
+      <c r="B22" s="66">
         <v>0.75</v>
       </c>
-      <c r="C22" s="35"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1601,9 +1601,9 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="29"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1619,9 +1619,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1638,9 +1638,9 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1657,11 +1657,11 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
-      <c r="B26" s="35">
+      <c r="A26" s="62"/>
+      <c r="B26" s="66">
         <v>0.5</v>
       </c>
-      <c r="C26" s="35"/>
+      <c r="C26" s="66"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1678,9 +1678,9 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1697,9 +1697,9 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1716,9 +1716,9 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1735,11 +1735,11 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="29"/>
-      <c r="B30" s="35">
+      <c r="A30" s="62"/>
+      <c r="B30" s="66">
         <v>0.25</v>
       </c>
-      <c r="C30" s="35"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1756,9 +1756,9 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="29"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1775,9 +1775,9 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1794,9 +1794,9 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1813,13 +1813,13 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="68">
         <v>0.1</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="68">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1838,9 +1838,9 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1857,9 +1857,9 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="32"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1876,9 +1876,9 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="33"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1895,14 +1895,14 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="47"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1916,12 +1916,12 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="33"/>
-      <c r="B39" s="39" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="15">
         <v>42.128999999999998</v>
       </c>
@@ -1935,13 +1935,13 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="53"/>
+      <c r="C40" s="56"/>
       <c r="D40" s="4" t="s">
         <v>16</v>
       </c>
@@ -1959,9 +1959,9 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="32"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="54"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="57"/>
       <c r="D41" s="6" t="s">
         <v>15</v>
       </c>
@@ -1979,11 +1979,11 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
-      <c r="B42" s="48" t="s">
+      <c r="A42" s="44"/>
+      <c r="B42" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="52"/>
       <c r="D42" s="6" t="s">
         <v>16</v>
       </c>
@@ -2001,9 +2001,9 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="54"/>
       <c r="D43" s="8" t="s">
         <v>15</v>
       </c>
@@ -2021,14 +2021,14 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="41"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -2042,12 +2042,12 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="33"/>
-      <c r="B45" s="39" t="s">
+      <c r="A45" s="43"/>
+      <c r="B45" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
       <c r="E45" s="15">
         <v>42.606000000000002</v>
       </c>
@@ -2061,12 +2061,12 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2092,13 +2092,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2115,6 +2108,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2126,7 +2126,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2208,22 +2208,22 @@
       <c r="G2" s="16">
         <v>0.48980000000000001</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="25">
         <v>0.7319</v>
       </c>
-      <c r="I2" s="66">
+      <c r="I2" s="25">
         <v>1212</v>
       </c>
-      <c r="J2" s="66">
+      <c r="J2" s="25">
         <v>0.73609999999999998</v>
       </c>
-      <c r="K2" s="66">
+      <c r="K2" s="25">
         <v>1219</v>
       </c>
-      <c r="L2" s="66">
+      <c r="L2" s="25">
         <v>0.73609999999999998</v>
       </c>
-      <c r="M2" s="66">
+      <c r="M2" s="25">
         <v>1219</v>
       </c>
     </row>
@@ -2249,22 +2249,22 @@
       <c r="G3" s="17">
         <v>0.4894</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="26">
         <v>0.69689999999999996</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="26">
         <v>1154</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="26">
         <v>0.70169999999999999</v>
       </c>
-      <c r="K3" s="67">
+      <c r="K3" s="26">
         <v>1162</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="26">
         <v>0.75119999999999998</v>
       </c>
-      <c r="M3" s="67">
+      <c r="M3" s="26">
         <v>1244</v>
       </c>
     </row>
@@ -2290,22 +2290,22 @@
       <c r="G4" s="17">
         <v>0.4723</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="27">
         <v>0.69930000000000003</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="27">
         <v>1158</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="27">
         <v>0.70409999999999995</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="27">
         <v>1166</v>
       </c>
-      <c r="L4" s="68">
+      <c r="L4" s="27">
         <v>0.75660000000000005</v>
       </c>
-      <c r="M4" s="68">
+      <c r="M4" s="27">
         <v>1253</v>
       </c>
     </row>
@@ -2331,22 +2331,22 @@
       <c r="G5" s="17">
         <v>0.4834</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="27">
         <v>0.69499999999999995</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="27">
         <v>1151</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="27">
         <v>0.69930000000000003</v>
       </c>
-      <c r="K5" s="68">
+      <c r="K5" s="27">
         <v>1158</v>
       </c>
-      <c r="L5" s="68">
+      <c r="L5" s="27">
         <v>0.74460000000000004</v>
       </c>
-      <c r="M5" s="68">
+      <c r="M5" s="27">
         <v>1233</v>
       </c>
     </row>
@@ -2372,22 +2372,22 @@
       <c r="G6" s="17">
         <v>0.49020000000000002</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="27">
         <v>0.68479999999999996</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="27">
         <v>1134</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="27">
         <v>0.68899999999999995</v>
       </c>
-      <c r="K6" s="68">
+      <c r="K6" s="27">
         <v>1141</v>
       </c>
-      <c r="L6" s="68">
+      <c r="L6" s="27">
         <v>0.73009999999999997</v>
       </c>
-      <c r="M6" s="68">
+      <c r="M6" s="27">
         <v>1209</v>
       </c>
     </row>
@@ -2401,157 +2401,157 @@
       <c r="C7" s="21">
         <v>43.001100000000001</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="36">
         <v>33.6</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="36">
         <v>52.72</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="36">
         <v>69.66</v>
       </c>
-      <c r="G7" s="77">
+      <c r="G7" s="36">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="28">
         <v>0.69810000000000005</v>
       </c>
-      <c r="I7" s="69">
+      <c r="I7" s="28">
         <v>1156</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="28">
         <v>0.70230000000000004</v>
       </c>
-      <c r="K7" s="69">
+      <c r="K7" s="28">
         <v>1163</v>
       </c>
-      <c r="L7" s="69">
+      <c r="L7" s="28">
         <v>0.75060000000000004</v>
       </c>
-      <c r="M7" s="69">
+      <c r="M7" s="28">
         <v>1243</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="34">
         <v>42.997799999999998</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="35">
         <v>33.450000000000003</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="35">
         <v>52.55</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="35">
         <v>69.88</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="35">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="35">
         <v>0.69440000000000002</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="35">
         <v>1150</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="35">
         <v>0.69930000000000003</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="35">
         <v>1158</v>
       </c>
-      <c r="L8" s="76">
+      <c r="L8" s="35">
         <v>0.74519999999999997</v>
       </c>
-      <c r="M8" s="76">
+      <c r="M8" s="35">
         <v>1234</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="74">
+      <c r="C9" s="33">
         <v>42.688000000000002</v>
       </c>
-      <c r="D9" s="74">
+      <c r="D9" s="33">
         <v>33.4</v>
       </c>
-      <c r="E9" s="74">
+      <c r="E9" s="33">
         <v>52.61</v>
       </c>
-      <c r="F9" s="74">
+      <c r="F9" s="33">
         <v>69.459999999999994</v>
       </c>
-      <c r="G9" s="74">
+      <c r="G9" s="33">
         <v>0.48449999999999999</v>
       </c>
-      <c r="H9" s="74">
+      <c r="H9" s="33">
         <v>0.69689999999999996</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="33">
         <v>1154</v>
       </c>
-      <c r="J9" s="74">
+      <c r="J9" s="33">
         <v>0.70109999999999995</v>
       </c>
-      <c r="K9" s="74">
+      <c r="K9" s="33">
         <v>1161</v>
       </c>
-      <c r="L9" s="74">
+      <c r="L9" s="33">
         <v>0.75119999999999998</v>
       </c>
-      <c r="M9" s="71">
+      <c r="M9" s="30">
         <v>1244</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="32">
         <v>42.839799999999997</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="31">
         <v>34.11</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="31">
         <v>53.06</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="31">
         <v>68.42</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="31">
         <v>0.4894</v>
       </c>
-      <c r="H10" s="72">
+      <c r="H10" s="31">
         <v>0.69630000000000003</v>
       </c>
-      <c r="I10" s="72">
+      <c r="I10" s="31">
         <v>1153</v>
       </c>
-      <c r="J10" s="72">
+      <c r="J10" s="31">
         <v>0.70109999999999995</v>
       </c>
-      <c r="K10" s="72">
+      <c r="K10" s="31">
         <v>1161</v>
       </c>
-      <c r="L10" s="72">
+      <c r="L10" s="31">
         <v>0.75119999999999998</v>
       </c>
-      <c r="M10" s="72">
+      <c r="M10" s="31">
         <v>1244</v>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="70" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="5">
@@ -2603,99 +2603,99 @@
       <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="58"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="74"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="64"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="7">
         <v>35.5</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="60"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="77"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="64"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="60"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="77"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="64"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="7">
         <v>35.18</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="60"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="7">
         <v>31.63</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="63"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2712,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2988,116 +2988,116 @@
       <c r="C7" s="9">
         <v>43.105200000000004</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="36">
         <v>33.86</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="36">
         <v>53.03</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="36">
         <v>68.69</v>
       </c>
-      <c r="G7" s="77">
+      <c r="G7" s="36">
         <v>0.51370000000000005</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="36">
         <v>0.75790000000000002</v>
       </c>
-      <c r="I7" s="77">
+      <c r="I7" s="36">
         <v>1255</v>
       </c>
-      <c r="J7" s="77">
+      <c r="J7" s="36">
         <v>0.76029999999999998</v>
       </c>
-      <c r="K7" s="77">
+      <c r="K7" s="36">
         <v>1259</v>
       </c>
-      <c r="L7" s="77">
+      <c r="L7" s="36">
         <v>0.76029999999999998</v>
       </c>
-      <c r="M7" s="77">
+      <c r="M7" s="36">
         <v>1259</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="34">
         <v>43.406100000000002</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="35">
         <v>33.82</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="35">
         <v>53.02</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="35">
         <v>68.540000000000006</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="35">
         <v>0.52449999999999997</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="35">
         <v>0.74209999999999998</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="35">
         <v>1229</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="35">
         <v>0.74580000000000002</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="35">
         <v>1235</v>
       </c>
-      <c r="L8" s="76">
+      <c r="L8" s="35">
         <v>0.74580000000000002</v>
       </c>
-      <c r="M8" s="76">
+      <c r="M8" s="35">
         <v>1235</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="37">
         <v>43.305199999999999</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="29">
         <v>34.299999999999997</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="29">
         <v>53.32</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="29">
         <v>67.87</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="29">
         <v>0.52629999999999999</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="29">
         <v>0.76329999999999998</v>
       </c>
-      <c r="I9" s="70">
+      <c r="I9" s="29">
         <v>1264</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="29">
         <v>0.76629999999999998</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="29">
         <v>1269</v>
       </c>
-      <c r="L9" s="70">
+      <c r="L9" s="29">
         <v>0.76629999999999998</v>
       </c>
-      <c r="M9" s="70">
+      <c r="M9" s="29">
         <v>1269</v>
       </c>
     </row>
@@ -3108,7 +3108,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="70" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3149,99 +3149,99 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="60"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="64"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="60"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="77"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="64"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="60"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="77"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3273,8 +3273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AE9F30-CD4B-42DC-84E4-E64EA556D182}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3385,34 +3385,34 @@
       <c r="C3" s="7">
         <v>40.444299999999998</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="26">
         <v>32.83</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="26">
         <v>52</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="26">
         <v>69.88</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="26">
         <v>0.51090000000000002</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="26">
         <v>0.72950000000000004</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="26">
         <v>1208</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="26">
         <v>0.73370000000000002</v>
       </c>
-      <c r="K3" s="67">
+      <c r="K3" s="26">
         <v>1215</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="26">
         <v>0.73370000000000002</v>
       </c>
-      <c r="M3" s="67">
+      <c r="M3" s="26">
         <v>1215</v>
       </c>
     </row>
@@ -3426,34 +3426,34 @@
       <c r="C4" s="7">
         <v>38.722200000000001</v>
       </c>
-      <c r="D4" s="67">
+      <c r="D4" s="26">
         <v>31.47</v>
       </c>
-      <c r="E4" s="67">
+      <c r="E4" s="26">
         <v>50.74</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="26">
         <v>71.33</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="26">
         <v>0.4773</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="26">
         <v>0.69630000000000003</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="26">
         <v>1153</v>
       </c>
-      <c r="J4" s="67">
+      <c r="J4" s="26">
         <v>0.70050000000000001</v>
       </c>
-      <c r="K4" s="67">
+      <c r="K4" s="26">
         <v>1160</v>
       </c>
-      <c r="L4" s="67">
+      <c r="L4" s="26">
         <v>0.70050000000000001</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M4" s="26">
         <v>1160</v>
       </c>
     </row>
@@ -3467,34 +3467,34 @@
       <c r="C5" s="7">
         <v>40.642400000000002</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="26">
         <v>32.68</v>
       </c>
-      <c r="E5" s="67">
+      <c r="E5" s="26">
         <v>51.81</v>
       </c>
-      <c r="F5" s="67">
+      <c r="F5" s="26">
         <v>69.739999999999995</v>
       </c>
-      <c r="G5" s="67">
+      <c r="G5" s="26">
         <v>0.51570000000000005</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="26">
         <v>0.72460000000000002</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="26">
         <v>1200</v>
       </c>
-      <c r="J5" s="67">
+      <c r="J5" s="26">
         <v>0.7319</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="26">
         <v>1212</v>
       </c>
-      <c r="L5" s="67">
+      <c r="L5" s="26">
         <v>0.7319</v>
       </c>
-      <c r="M5" s="67">
+      <c r="M5" s="26">
         <v>1212</v>
       </c>
     </row>
@@ -3505,37 +3505,37 @@
       <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="80">
+      <c r="C6" s="38">
         <v>48.509300000000003</v>
       </c>
-      <c r="D6" s="67">
+      <c r="D6" s="26">
         <v>32.799999999999997</v>
       </c>
-      <c r="E6" s="67">
+      <c r="E6" s="26">
         <v>51.62</v>
       </c>
-      <c r="F6" s="67">
+      <c r="F6" s="26">
         <v>70.489999999999995</v>
       </c>
-      <c r="G6" s="67">
+      <c r="G6" s="26">
         <v>0.5141</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="26">
         <v>0.72519999999999996</v>
       </c>
-      <c r="I6" s="67">
+      <c r="I6" s="26">
         <v>1201</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="25">
         <v>0.72829999999999995</v>
       </c>
-      <c r="K6" s="66">
+      <c r="K6" s="25">
         <v>1206</v>
       </c>
-      <c r="L6" s="66">
+      <c r="L6" s="25">
         <v>0.72829999999999995</v>
       </c>
-      <c r="M6" s="67">
+      <c r="M6" s="26">
         <v>1206</v>
       </c>
     </row>
@@ -3549,116 +3549,116 @@
       <c r="C7" s="9">
         <v>40.878</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="36">
         <v>32.130000000000003</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="36">
         <v>51.44</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="36">
         <v>70.7</v>
       </c>
-      <c r="G7" s="77">
+      <c r="G7" s="36">
         <v>0.50939999999999996</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="36">
         <v>0.72709999999999997</v>
       </c>
-      <c r="I7" s="77">
+      <c r="I7" s="36">
         <v>1204</v>
       </c>
-      <c r="J7" s="77">
+      <c r="J7" s="36">
         <v>0.7319</v>
       </c>
-      <c r="K7" s="77">
+      <c r="K7" s="36">
         <v>1212</v>
       </c>
-      <c r="L7" s="77">
+      <c r="L7" s="36">
         <v>0.7319</v>
       </c>
-      <c r="M7" s="77">
+      <c r="M7" s="36">
         <v>1212</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="34">
         <v>40.930199999999999</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="35">
         <v>33.03</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="35">
         <v>52.01</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="35">
         <v>70.040000000000006</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="35">
         <v>0.51149999999999995</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="35">
         <v>0.72519999999999996</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="35">
         <v>1201</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="35">
         <v>0.72950000000000004</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="35">
         <v>1208</v>
       </c>
-      <c r="L8" s="76">
+      <c r="L8" s="35">
         <v>0.72950000000000004</v>
       </c>
-      <c r="M8" s="76">
+      <c r="M8" s="35">
         <v>1208</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="37">
         <v>40.607199999999999</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="29">
         <v>31.77</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="29">
         <v>51.23</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="29">
         <v>70.650000000000006</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="29">
         <v>0.50800000000000001</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="29">
         <v>0.72040000000000004</v>
       </c>
-      <c r="I9" s="70">
+      <c r="I9" s="29">
         <v>1193</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="29">
         <v>0.72399999999999998</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="29">
         <v>1199</v>
       </c>
-      <c r="L9" s="70">
+      <c r="L9" s="29">
         <v>0.72399999999999998</v>
       </c>
-      <c r="M9" s="70">
+      <c r="M9" s="29">
         <v>1199</v>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="70" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3710,99 +3710,99 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="60"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="64"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="60"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="77"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="64"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="60"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="77"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3821,6 +3821,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -4049,14 +4057,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4067,6 +4067,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4085,23 +4102,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add data analysis and rerun choi on m2m
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="837" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87C403F8-D412-4EFD-91CA-D1979274D602}"/>
+  <xr:revisionPtr revIDLastSave="855" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{520987FB-1783-4378-9A01-A3B3D330BD79}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2424" yWindow="0" windowWidth="20592" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
   <si>
     <t>Weight</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>OPUS-MT-TC-BIG-EN-FR</t>
-  </si>
-  <si>
-    <t>TBC</t>
   </si>
   <si>
     <t>WCE using best hyperparameters</t>
@@ -278,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,14 +300,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -583,24 +574,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,8 +689,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -723,24 +743,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -769,39 +771,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1124,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,13 +1134,13 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="45">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1197,9 +1166,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1215,7 +1184,7 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3">
-        <f>MEDIAN(E22:E33)</f>
+        <f>MEDIAN(E18:E29)</f>
         <v>42.64105</v>
       </c>
       <c r="J3" t="s">
@@ -1223,9 +1192,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1242,9 +1211,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1261,9 +1230,9 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66">
+      <c r="A6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1282,9 +1251,9 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1301,9 +1270,9 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1320,9 +1289,9 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1339,9 +1308,9 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66">
+      <c r="A10" s="39"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1354,15 +1323,15 @@
         <v>11230.0195</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" ref="G10:G21" si="1">F10*32.6*0.3 / 1000</f>
+        <f t="shared" ref="G10:G17" si="1">F10*32.6*0.3 / 1000</f>
         <v>109.82959071000001</v>
       </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1379,9 +1348,9 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1398,9 +1367,9 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1419,13 +1388,13 @@
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66">
+      <c r="A14" s="39"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1449,13 +1418,13 @@
         <v>25883.389200000001</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1472,9 +1441,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1491,9 +1460,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1510,611 +1479,540 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="62"/>
-      <c r="B18" s="58">
-        <v>1</v>
-      </c>
-      <c r="C18" s="66"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="46"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="19">
+        <v>42.6248</v>
+      </c>
+      <c r="F18" s="7">
+        <v>15649.238600000001</v>
+      </c>
       <c r="G18" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>54</v>
-      </c>
+        <f t="shared" ref="G18:G42" si="2">F18*32.6*0.3 / 1000</f>
+        <v>153.049553508</v>
+      </c>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="62"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="66"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="19">
+        <v>42.568800000000003</v>
+      </c>
+      <c r="F19" s="7">
+        <v>15634.0206</v>
+      </c>
       <c r="G19" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>54</v>
+        <f t="shared" si="2"/>
+        <v>152.900721468</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="62"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="66"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="19">
+        <v>42.657299999999999</v>
+      </c>
+      <c r="F20" s="7">
+        <v>24736.3887</v>
+      </c>
       <c r="G20" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>54</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>241.92188148599999</v>
+      </c>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="62"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="66"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="19">
+        <v>42.586300000000001</v>
+      </c>
+      <c r="F21" s="7">
+        <v>25533.498100000001</v>
+      </c>
       <c r="G21" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>54</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>249.71761141800002</v>
+      </c>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="62"/>
-      <c r="B22" s="66">
-        <v>0.75</v>
-      </c>
-      <c r="C22" s="66"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="46"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
       <c r="E22" s="19">
-        <v>42.6248</v>
+        <v>42.834800000000001</v>
       </c>
       <c r="F22" s="7">
-        <v>15649.238600000001</v>
+        <v>22345.029500000001</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" ref="G22:G46" si="2">F22*32.6*0.3 / 1000</f>
-        <v>153.049553508</v>
+        <f t="shared" si="2"/>
+        <v>218.53438851000001</v>
       </c>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
       <c r="E23" s="19">
-        <v>42.568800000000003</v>
+        <v>42.8322</v>
       </c>
       <c r="F23" s="7">
-        <v>15634.0206</v>
+        <v>25586.411599999999</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="2"/>
-        <v>152.900721468</v>
-      </c>
+        <v>250.23510544799998</v>
+      </c>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
       <c r="E24" s="19">
-        <v>42.657299999999999</v>
+        <v>42.7468</v>
       </c>
       <c r="F24" s="7">
-        <v>24736.3887</v>
+        <v>25118.774000000001</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="2"/>
-        <v>241.92188148599999</v>
+        <v>245.66160972</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="62"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="19">
-        <v>42.586300000000001</v>
+        <v>42.115699999999997</v>
       </c>
       <c r="F25" s="7">
-        <v>25533.498100000001</v>
+        <v>15740.974700000001</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="2"/>
-        <v>249.71761141800002</v>
+        <v>153.94673256600001</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="62"/>
-      <c r="B26" s="66">
-        <v>0.5</v>
-      </c>
-      <c r="C26" s="66"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="C26" s="46"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
       <c r="E26" s="19">
-        <v>42.834800000000001</v>
+        <v>42.577399999999997</v>
       </c>
       <c r="F26" s="7">
-        <v>22345.029500000001</v>
+        <v>15012.536</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="2"/>
-        <v>218.53438851000001</v>
+        <v>146.82260208000002</v>
       </c>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="62"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
-      <c r="E27" s="19">
-        <v>42.8322</v>
+      <c r="E27" s="23">
+        <v>42.997799999999998</v>
       </c>
       <c r="F27" s="7">
-        <v>25586.411599999999</v>
+        <v>24740.625</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" si="2"/>
-        <v>250.23510544799998</v>
+        <v>241.9633125</v>
       </c>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="62"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
       <c r="E28" s="19">
-        <v>42.7468</v>
+        <v>42.590800000000002</v>
       </c>
       <c r="F28" s="7">
-        <v>25118.774000000001</v>
+        <v>24592.9486</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="2"/>
-        <v>245.66160972</v>
+        <v>240.51903730800001</v>
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="62"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="6">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="40"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="8">
         <v>2</v>
       </c>
-      <c r="E29" s="19">
-        <v>42.115699999999997</v>
-      </c>
-      <c r="F29" s="7">
-        <v>15740.974700000001</v>
-      </c>
-      <c r="G29" s="7">
+      <c r="E29" s="21">
+        <v>42.779699999999998</v>
+      </c>
+      <c r="F29" s="9">
+        <v>24985.3393</v>
+      </c>
+      <c r="G29" s="9">
         <f t="shared" si="2"/>
-        <v>153.94673256600001</v>
+        <v>244.35661835400001</v>
       </c>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="62"/>
-      <c r="B30" s="66">
-        <v>0.25</v>
-      </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="6">
+      <c r="A30" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="C30" s="48">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
         <v>1.25</v>
       </c>
-      <c r="E30" s="19">
-        <v>42.577399999999997</v>
-      </c>
-      <c r="F30" s="7">
-        <v>15012.536</v>
-      </c>
-      <c r="G30" s="7">
+      <c r="E30" s="22">
+        <v>43.001100000000001</v>
+      </c>
+      <c r="F30" s="5">
+        <v>25190.439699999999</v>
+      </c>
+      <c r="G30" s="5">
         <f t="shared" si="2"/>
-        <v>146.82260208000002</v>
+        <v>246.36250026599998</v>
       </c>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="62"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
-      <c r="E31" s="23">
-        <v>42.997799999999998</v>
+      <c r="E31" s="19">
+        <v>42.782299999999999</v>
       </c>
       <c r="F31" s="7">
-        <v>24740.625</v>
+        <v>20479.9146</v>
       </c>
       <c r="G31" s="7">
         <f t="shared" si="2"/>
-        <v>241.9633125</v>
+        <v>200.29356478800003</v>
       </c>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="62"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
       <c r="E32" s="19">
-        <v>42.590800000000002</v>
+        <v>42.821300000000001</v>
       </c>
       <c r="F32" s="7">
-        <v>24592.9486</v>
+        <v>25430.924900000002</v>
       </c>
       <c r="G32" s="7">
         <f t="shared" si="2"/>
-        <v>240.51903730800001</v>
+        <v>248.71444552200003</v>
       </c>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="63"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="43"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
       <c r="E33" s="21">
-        <v>42.779699999999998</v>
+        <v>41.998399999999997</v>
       </c>
       <c r="F33" s="9">
-        <v>24985.3393</v>
+        <v>15306.2101</v>
       </c>
       <c r="G33" s="9">
         <f t="shared" si="2"/>
-        <v>244.35661835400001</v>
+        <v>149.69473477800003</v>
       </c>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="68">
-        <v>0.1</v>
-      </c>
-      <c r="C34" s="68">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="E34" s="22">
-        <v>43.001100000000001</v>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="4">
+        <v>42.087400000000002</v>
       </c>
       <c r="F34" s="5">
-        <v>25190.439699999999</v>
+        <v>12104.798500000001</v>
       </c>
       <c r="G34" s="5">
         <f t="shared" si="2"/>
-        <v>246.36250026599998</v>
+        <v>118.38492933000002</v>
       </c>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="44"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E35" s="19">
-        <v>42.782299999999999</v>
-      </c>
-      <c r="F35" s="7">
-        <v>20479.9146</v>
-      </c>
-      <c r="G35" s="7">
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="43"/>
+      <c r="B35" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="15">
+        <v>42.128999999999998</v>
+      </c>
+      <c r="F35" s="9">
+        <v>9021.1026999999995</v>
+      </c>
+      <c r="G35" s="9">
         <f t="shared" si="2"/>
-        <v>200.29356478800003</v>
+        <v>88.226384405999994</v>
       </c>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="44"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="6">
-        <v>1.75</v>
-      </c>
-      <c r="E36" s="19">
-        <v>42.821300000000001</v>
-      </c>
-      <c r="F36" s="7">
-        <v>25430.924900000002</v>
-      </c>
-      <c r="G36" s="7">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="64"/>
+      <c r="D36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="4">
+        <v>41.673900000000003</v>
+      </c>
+      <c r="F36" s="5">
+        <f>F42 + 815.0048</f>
+        <v>18004.647499999999</v>
+      </c>
+      <c r="G36" s="5">
         <f t="shared" si="2"/>
-        <v>248.71444552200003</v>
+        <v>176.08545254999999</v>
       </c>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="43"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="8">
-        <v>2</v>
-      </c>
-      <c r="E37" s="21">
-        <v>41.998399999999997</v>
-      </c>
-      <c r="F37" s="9">
-        <v>15306.2101</v>
-      </c>
-      <c r="G37" s="9">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="42"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="6">
+        <v>38.872199999999999</v>
+      </c>
+      <c r="F37" s="7">
+        <f>F42 + 1547.1448</f>
+        <v>18736.787499999999</v>
+      </c>
+      <c r="G37" s="7">
         <f t="shared" si="2"/>
-        <v>149.69473477800003</v>
+        <v>183.24578174999999</v>
       </c>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="4">
-        <v>42.087400000000002</v>
-      </c>
-      <c r="F38" s="5">
-        <v>12104.798500000001</v>
-      </c>
-      <c r="G38" s="5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="42"/>
+      <c r="B38" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="13">
+        <v>41.738300000000002</v>
+      </c>
+      <c r="F38" s="7">
+        <f>F42 + 859.7958</f>
+        <v>18049.4385</v>
+      </c>
+      <c r="G38" s="7">
         <f t="shared" si="2"/>
-        <v>118.38492933000002</v>
+        <v>176.52350852999999</v>
       </c>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="43"/>
-      <c r="B39" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="15">
-        <v>42.128999999999998</v>
+      <c r="B39" s="61"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="8">
+        <v>40.942300000000003</v>
       </c>
       <c r="F39" s="9">
-        <v>9021.1026999999995</v>
+        <f>F42 + 1529.7841</f>
+        <v>18719.426800000001</v>
       </c>
       <c r="G39" s="9">
         <f t="shared" si="2"/>
-        <v>88.226384405999994</v>
+        <v>183.07599410400002</v>
       </c>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="55" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="4">
-        <v>41.673900000000003</v>
+        <v>42.231000000000002</v>
       </c>
       <c r="F40" s="5">
-        <f>F46 + 815.0048</f>
-        <v>18004.647499999999</v>
+        <v>13749.5393</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="2"/>
-        <v>176.08545254999999</v>
+        <v>134.47049435399998</v>
       </c>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="44"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="6">
-        <v>38.872199999999999</v>
-      </c>
-      <c r="F41" s="7">
-        <f>F46 + 1547.1448</f>
-        <v>18736.787499999999</v>
-      </c>
-      <c r="G41" s="7">
-        <f t="shared" si="2"/>
-        <v>183.24578174999999</v>
-      </c>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
-      <c r="B42" s="51" t="s">
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="43"/>
+      <c r="B41" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="13">
-        <v>41.738300000000002</v>
-      </c>
-      <c r="F42" s="7">
-        <f>F46 + 859.7958</f>
-        <v>18049.4385</v>
-      </c>
-      <c r="G42" s="7">
-        <f t="shared" si="2"/>
-        <v>176.52350852999999</v>
-      </c>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="43" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="43"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="8">
-        <v>40.942300000000003</v>
-      </c>
-      <c r="F43" s="9">
-        <f>F46 + 1529.7841</f>
-        <v>18719.426800000001</v>
-      </c>
-      <c r="G43" s="9">
-        <f t="shared" si="2"/>
-        <v>183.07599410400002</v>
-      </c>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="40"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="4">
-        <v>42.231000000000002</v>
-      </c>
-      <c r="F44" s="5">
-        <v>13749.5393</v>
-      </c>
-      <c r="G44" s="5">
-        <f t="shared" si="2"/>
-        <v>134.47049435399998</v>
-      </c>
-      <c r="H44" s="10"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="43"/>
-      <c r="B45" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="15">
+      <c r="C41" s="51"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="15">
         <v>42.606000000000002</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F41" s="9">
         <v>8859.1144999999997</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G41" s="9">
         <f t="shared" si="2"/>
         <v>86.642139810000003</v>
       </c>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="65" t="s">
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="5">
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="5">
         <v>42.67</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F42" s="5">
         <v>17189.6427</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G42" s="5">
         <f t="shared" si="2"/>
         <v>168.114705606</v>
       </c>
-      <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="52" spans="12:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L52" s="12"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L48" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A46:D46"/>
+  <mergeCells count="22">
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="A2:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A42:D42"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C33"/>
+    <mergeCell ref="C14:C29"/>
+    <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2125,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,19 +2069,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2437,7 +2335,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="34">
         <v>42.997799999999998</v>
@@ -2475,10 +2373,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="33">
         <v>42.688000000000002</v>
@@ -2516,10 +2414,10 @@
     </row>
     <row r="10" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>60</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>61</v>
       </c>
       <c r="C10" s="32">
         <v>42.839799999999997</v>
@@ -2562,7 +2460,7 @@
       <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="67" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="5">
@@ -2603,99 +2501,99 @@
       <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="74"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="7">
         <v>35.5</v>
       </c>
-      <c r="E13" s="75"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="77"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="77"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="74"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="7">
         <v>35.18</v>
       </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="77"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="74"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="71"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="7">
         <v>31.63</v>
       </c>
-      <c r="E16" s="78"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="80"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2712,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,19 +2656,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -3024,7 +2922,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="34">
         <v>43.406100000000002</v>
@@ -3062,10 +2960,10 @@
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="37">
         <v>43.305199999999999</v>
@@ -3108,7 +3006,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="67" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3149,99 +3047,99 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="74"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="77"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="74"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="75"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="77"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="77"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="74"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="80"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3274,7 +3172,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C6" sqref="C6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3319,19 +3217,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -3339,7 +3237,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>52</v>
@@ -3505,38 +3403,38 @@
       <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="38">
-        <v>48.509300000000003</v>
+      <c r="C6" s="27">
+        <v>40.634</v>
       </c>
       <c r="D6" s="26">
-        <v>32.799999999999997</v>
+        <v>33.090000000000003</v>
       </c>
       <c r="E6" s="26">
-        <v>51.62</v>
+        <v>51.98</v>
       </c>
       <c r="F6" s="26">
-        <v>70.489999999999995</v>
+        <v>69.52</v>
       </c>
       <c r="G6" s="26">
-        <v>0.5141</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="H6" s="26">
-        <v>0.72519999999999996</v>
+        <v>0.7198</v>
       </c>
       <c r="I6" s="26">
-        <v>1201</v>
+        <v>1192</v>
       </c>
       <c r="J6" s="25">
-        <v>0.72829999999999995</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="K6" s="25">
-        <v>1206</v>
+        <v>1199</v>
       </c>
       <c r="L6" s="25">
-        <v>0.72829999999999995</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="M6" s="26">
-        <v>1206</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3585,7 +3483,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="34">
         <v>40.930199999999999</v>
@@ -3623,10 +3521,10 @@
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="37">
         <v>40.607199999999999</v>
@@ -3669,7 +3567,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="67" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3710,99 +3608,99 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="74"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="77"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="74"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="75"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="77"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="77"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="74"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="80"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3821,14 +3719,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -4057,6 +3947,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4067,23 +3965,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4102,6 +3983,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Incorporate Stanza NER and NCBO Ontologies in term list
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -689,6 +689,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,12 +749,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,18 +764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,36 +772,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1134,13 +1134,13 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="59">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1166,9 +1166,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1192,9 +1192,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1211,9 +1211,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1230,9 +1230,9 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46">
+      <c r="A6" s="55"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1251,9 +1251,9 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1270,9 +1270,9 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1289,9 +1289,9 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1308,9 +1308,9 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46">
+      <c r="A10" s="55"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1329,9 +1329,9 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1348,9 +1348,9 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1367,9 +1367,9 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1392,9 +1392,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46">
+      <c r="A14" s="55"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1422,9 +1422,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1441,9 +1441,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1460,9 +1460,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1479,11 +1479,11 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="46">
+      <c r="A18" s="55"/>
+      <c r="B18" s="60">
         <v>0.75</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1500,9 +1500,9 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1518,9 +1518,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1537,9 +1537,9 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1556,11 +1556,11 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="46">
+      <c r="A22" s="55"/>
+      <c r="B22" s="60">
         <v>0.5</v>
       </c>
-      <c r="C22" s="46"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1577,9 +1577,9 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1596,9 +1596,9 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1615,9 +1615,9 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1634,11 +1634,11 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
-      <c r="B26" s="46">
+      <c r="A26" s="55"/>
+      <c r="B26" s="60">
         <v>0.25</v>
       </c>
-      <c r="C26" s="46"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1655,9 +1655,9 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1674,9 +1674,9 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1693,9 +1693,9 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="8">
         <v>2</v>
       </c>
@@ -1712,13 +1712,13 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="62">
         <v>0.1</v>
       </c>
-      <c r="C30" s="48">
+      <c r="C30" s="62">
         <v>1</v>
       </c>
       <c r="D30" s="4">
@@ -1737,9 +1737,9 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1756,9 +1756,9 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1775,9 +1775,9 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="43"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1794,14 +1794,14 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1815,12 +1815,12 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43"/>
-      <c r="B35" s="50" t="s">
+      <c r="A35" s="39"/>
+      <c r="B35" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="15">
         <v>42.128999999999998</v>
       </c>
@@ -1834,13 +1834,13 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="64"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="4" t="s">
         <v>16</v>
       </c>
@@ -1858,9 +1858,9 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="65"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="53"/>
       <c r="D37" s="6" t="s">
         <v>15</v>
       </c>
@@ -1878,11 +1878,11 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="59" t="s">
+      <c r="A38" s="40"/>
+      <c r="B38" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="60"/>
+      <c r="C38" s="48"/>
       <c r="D38" s="6" t="s">
         <v>16</v>
       </c>
@@ -1900,9 +1900,9 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="43"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="62"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="8" t="s">
         <v>15</v>
       </c>
@@ -1920,14 +1920,14 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1941,12 +1941,12 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="43"/>
-      <c r="B41" s="50" t="s">
+      <c r="A41" s="39"/>
+      <c r="B41" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="43"/>
       <c r="E41" s="15">
         <v>42.606000000000002</v>
       </c>
@@ -1960,12 +1960,12 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="5">
         <v>42.67</v>
       </c>
@@ -1991,12 +1991,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="B36:C37"/>
     <mergeCell ref="A2:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A42:D42"/>
@@ -2013,6 +2007,12 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B36:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2024,7 +2024,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,7 +2611,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3719,6 +3719,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -3947,14 +3955,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3965,6 +3965,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3983,23 +4000,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update results for new term list
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="855" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{520987FB-1783-4378-9A01-A3B3D330BD79}"/>
+  <xr:revisionPtr revIDLastSave="1053" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFCDCC7E-EAC5-4CD5-A0A8-EBDAD967CE04}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="0" windowWidth="20592" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -237,6 +237,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,15 +692,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -708,6 +738,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -737,42 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -808,6 +811,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -1134,13 +1143,13 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="59">
+      <c r="C2" s="45">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1166,9 +1175,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1192,9 +1201,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1211,9 +1220,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1230,9 +1239,9 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60">
+      <c r="A6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1251,9 +1260,9 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1270,9 +1279,9 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1289,9 +1298,9 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1308,9 +1317,9 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60">
+      <c r="A10" s="39"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1329,9 +1338,9 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1348,9 +1357,9 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1367,9 +1376,9 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="55"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1392,9 +1401,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60">
+      <c r="A14" s="39"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1422,9 +1431,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1441,9 +1450,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1460,9 +1469,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1479,11 +1488,11 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
-      <c r="B18" s="60">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <v>0.75</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1500,9 +1509,9 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="55"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1518,9 +1527,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="55"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1537,9 +1546,9 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1556,11 +1565,11 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
-      <c r="B22" s="60">
+      <c r="A22" s="39"/>
+      <c r="B22" s="46">
         <v>0.5</v>
       </c>
-      <c r="C22" s="60"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1577,9 +1586,9 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1596,9 +1605,9 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1615,9 +1624,9 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1634,11 +1643,11 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
-      <c r="B26" s="60">
+      <c r="A26" s="39"/>
+      <c r="B26" s="46">
         <v>0.25</v>
       </c>
-      <c r="C26" s="60"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1655,9 +1664,9 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1674,9 +1683,9 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1693,9 +1702,9 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="8">
         <v>2</v>
       </c>
@@ -1712,13 +1721,13 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="62">
+      <c r="B30" s="48">
         <v>0.1</v>
       </c>
-      <c r="C30" s="62">
+      <c r="C30" s="48">
         <v>1</v>
       </c>
       <c r="D30" s="4">
@@ -1737,9 +1746,9 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1756,9 +1765,9 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1775,9 +1784,9 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1794,14 +1803,14 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="46"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
       <c r="E34" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1815,12 +1824,12 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="39"/>
-      <c r="B35" s="41" t="s">
+      <c r="A35" s="43"/>
+      <c r="B35" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="15">
         <v>42.128999999999998</v>
       </c>
@@ -1834,13 +1843,13 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="52"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="4" t="s">
         <v>16</v>
       </c>
@@ -1858,9 +1867,9 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="53"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="65"/>
       <c r="D37" s="6" t="s">
         <v>15</v>
       </c>
@@ -1878,11 +1887,11 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
-      <c r="B38" s="47" t="s">
+      <c r="A38" s="42"/>
+      <c r="B38" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="48"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="6" t="s">
         <v>16</v>
       </c>
@@ -1900,9 +1909,9 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="39"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="50"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="62"/>
       <c r="D39" s="8" t="s">
         <v>15</v>
       </c>
@@ -1920,14 +1929,14 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="65"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1941,12 +1950,12 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="39"/>
-      <c r="B41" s="41" t="s">
+      <c r="A41" s="43"/>
+      <c r="B41" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="43"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="52"/>
       <c r="E41" s="15">
         <v>42.606000000000002</v>
       </c>
@@ -1960,12 +1969,12 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
       <c r="E42" s="5">
         <v>42.67</v>
       </c>
@@ -1991,6 +2000,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B36:C37"/>
     <mergeCell ref="A2:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A42:D42"/>
@@ -2007,12 +2022,6 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="B36:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2021,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,23 +2115,23 @@
       <c r="G2" s="16">
         <v>0.48980000000000001</v>
       </c>
-      <c r="H2" s="25">
-        <v>0.7319</v>
+      <c r="H2" s="78">
+        <v>0.72270000000000001</v>
       </c>
       <c r="I2" s="25">
-        <v>1212</v>
+        <v>1011</v>
       </c>
       <c r="J2" s="25">
-        <v>0.73609999999999998</v>
+        <v>0.72550000000000003</v>
       </c>
       <c r="K2" s="25">
-        <v>1219</v>
+        <v>1015</v>
       </c>
       <c r="L2" s="25">
-        <v>0.73609999999999998</v>
+        <v>0.72550000000000003</v>
       </c>
       <c r="M2" s="25">
-        <v>1219</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2148,22 +2157,22 @@
         <v>0.4894</v>
       </c>
       <c r="H3" s="26">
-        <v>0.69689999999999996</v>
+        <v>0.68620000000000003</v>
       </c>
       <c r="I3" s="26">
-        <v>1154</v>
+        <v>960</v>
       </c>
       <c r="J3" s="26">
-        <v>0.70169999999999999</v>
+        <v>0.68910000000000005</v>
       </c>
       <c r="K3" s="26">
-        <v>1162</v>
+        <v>964</v>
       </c>
       <c r="L3" s="26">
-        <v>0.75119999999999998</v>
+        <v>0.74550000000000005</v>
       </c>
       <c r="M3" s="26">
-        <v>1244</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2189,22 +2198,22 @@
         <v>0.4723</v>
       </c>
       <c r="H4" s="27">
-        <v>0.69930000000000003</v>
+        <v>0.67410000000000003</v>
       </c>
       <c r="I4" s="27">
-        <v>1158</v>
+        <v>943</v>
       </c>
       <c r="J4" s="27">
-        <v>0.70409999999999995</v>
+        <v>0.67759999999999998</v>
       </c>
       <c r="K4" s="27">
-        <v>1166</v>
+        <v>948</v>
       </c>
       <c r="L4" s="27">
-        <v>0.75660000000000005</v>
+        <v>0.74409999999999998</v>
       </c>
       <c r="M4" s="27">
-        <v>1253</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2230,22 +2239,22 @@
         <v>0.4834</v>
       </c>
       <c r="H5" s="27">
-        <v>0.69499999999999995</v>
+        <v>0.67479999999999996</v>
       </c>
       <c r="I5" s="27">
-        <v>1151</v>
+        <v>944</v>
       </c>
       <c r="J5" s="27">
-        <v>0.69930000000000003</v>
+        <v>0.67759999999999998</v>
       </c>
       <c r="K5" s="27">
-        <v>1158</v>
+        <v>948</v>
       </c>
       <c r="L5" s="27">
-        <v>0.74460000000000004</v>
+        <v>0.74339999999999995</v>
       </c>
       <c r="M5" s="27">
-        <v>1233</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2271,22 +2280,22 @@
         <v>0.49020000000000002</v>
       </c>
       <c r="H6" s="27">
-        <v>0.68479999999999996</v>
+        <v>0.67479999999999996</v>
       </c>
       <c r="I6" s="27">
-        <v>1134</v>
+        <v>944</v>
       </c>
       <c r="J6" s="27">
-        <v>0.68899999999999995</v>
+        <v>0.67689999999999995</v>
       </c>
       <c r="K6" s="27">
-        <v>1141</v>
+        <v>947</v>
       </c>
       <c r="L6" s="27">
-        <v>0.73009999999999997</v>
+        <v>0.73480000000000001</v>
       </c>
       <c r="M6" s="27">
-        <v>1209</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2312,22 +2321,22 @@
         <v>0.48559999999999998</v>
       </c>
       <c r="H7" s="28">
-        <v>0.69810000000000005</v>
+        <v>0.6905</v>
       </c>
       <c r="I7" s="28">
-        <v>1156</v>
+        <v>966</v>
       </c>
       <c r="J7" s="28">
-        <v>0.70230000000000004</v>
+        <v>0.69410000000000005</v>
       </c>
       <c r="K7" s="28">
-        <v>1163</v>
+        <v>971</v>
       </c>
       <c r="L7" s="28">
-        <v>0.75060000000000004</v>
+        <v>0.75270000000000004</v>
       </c>
       <c r="M7" s="28">
-        <v>1243</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2353,22 +2362,22 @@
         <v>0.48559999999999998</v>
       </c>
       <c r="H8" s="35">
-        <v>0.69440000000000002</v>
+        <v>0.68620000000000003</v>
       </c>
       <c r="I8" s="35">
-        <v>1150</v>
+        <v>960</v>
       </c>
       <c r="J8" s="35">
-        <v>0.69930000000000003</v>
+        <v>0.68979999999999997</v>
       </c>
       <c r="K8" s="35">
-        <v>1158</v>
+        <v>965</v>
       </c>
       <c r="L8" s="35">
-        <v>0.74519999999999997</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="M8" s="35">
-        <v>1234</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -2394,22 +2403,22 @@
         <v>0.48449999999999999</v>
       </c>
       <c r="H9" s="33">
-        <v>0.69689999999999996</v>
+        <v>0.68189999999999995</v>
       </c>
       <c r="I9" s="33">
-        <v>1154</v>
+        <v>954</v>
       </c>
       <c r="J9" s="33">
-        <v>0.70109999999999995</v>
+        <v>0.6855</v>
       </c>
       <c r="K9" s="33">
-        <v>1161</v>
+        <v>959</v>
       </c>
       <c r="L9" s="33">
-        <v>0.75119999999999998</v>
+        <v>0.74480000000000002</v>
       </c>
       <c r="M9" s="30">
-        <v>1244</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2435,22 +2444,22 @@
         <v>0.4894</v>
       </c>
       <c r="H10" s="31">
-        <v>0.69630000000000003</v>
+        <v>0.68479999999999996</v>
       </c>
       <c r="I10" s="31">
-        <v>1153</v>
+        <v>958</v>
       </c>
       <c r="J10" s="31">
-        <v>0.70109999999999995</v>
+        <v>0.68759999999999999</v>
       </c>
       <c r="K10" s="31">
-        <v>1161</v>
+        <v>962</v>
       </c>
       <c r="L10" s="31">
-        <v>0.75119999999999998</v>
+        <v>0.74480000000000002</v>
       </c>
       <c r="M10" s="31">
-        <v>1244</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2475,23 +2484,23 @@
       <c r="G11" s="5">
         <v>0.5131</v>
       </c>
-      <c r="H11" s="5">
-        <v>0.77359999999999995</v>
+      <c r="H11" s="79">
+        <v>0.76480000000000004</v>
       </c>
       <c r="I11" s="5">
-        <v>1281</v>
+        <v>1070</v>
       </c>
       <c r="J11" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="K11" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
       <c r="L11" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="M11" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2594,6 +2603,10 @@
       <c r="K16" s="76"/>
       <c r="L16" s="76"/>
       <c r="M16" s="77"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2610,8 +2623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2694,22 +2707,22 @@
         <v>0.50900000000000001</v>
       </c>
       <c r="H2" s="16">
-        <v>0.76390000000000002</v>
+        <v>0.75480000000000003</v>
       </c>
       <c r="I2" s="16">
-        <v>1265</v>
+        <v>1056</v>
       </c>
       <c r="J2" s="16">
-        <v>0.76690000000000003</v>
+        <v>0.75839999999999996</v>
       </c>
       <c r="K2" s="16">
-        <v>1270</v>
+        <v>1061</v>
       </c>
       <c r="L2" s="16">
-        <v>0.76690000000000003</v>
+        <v>0.75839999999999996</v>
       </c>
       <c r="M2" s="16">
-        <v>1270</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2735,22 +2748,22 @@
         <v>0.52349999999999997</v>
       </c>
       <c r="H3" s="17">
-        <v>0.753</v>
+        <v>0.75409999999999999</v>
       </c>
       <c r="I3" s="17">
-        <v>1247</v>
+        <v>1055</v>
       </c>
       <c r="J3" s="17">
-        <v>0.75539999999999996</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="K3" s="17">
-        <v>1251</v>
+        <v>1059</v>
       </c>
       <c r="L3" s="17">
-        <v>0.75539999999999996</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="M3" s="17">
-        <v>1251</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2776,22 +2789,22 @@
         <v>0.52090000000000003</v>
       </c>
       <c r="H4" s="17">
-        <v>0.74460000000000004</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="I4" s="17">
-        <v>1233</v>
+        <v>1046</v>
       </c>
       <c r="J4" s="17">
-        <v>0.74880000000000002</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="K4" s="17">
-        <v>1240</v>
+        <v>1050</v>
       </c>
       <c r="L4" s="17">
-        <v>0.74880000000000002</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="M4" s="17">
-        <v>1240</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2817,22 +2830,22 @@
         <v>0.52569999999999995</v>
       </c>
       <c r="H5" s="17">
-        <v>0.74580000000000002</v>
+        <v>0.74480000000000002</v>
       </c>
       <c r="I5" s="17">
-        <v>1235</v>
+        <v>1042</v>
       </c>
       <c r="J5" s="17">
-        <v>0.74939999999999996</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="K5" s="17">
-        <v>1241</v>
+        <v>1046</v>
       </c>
       <c r="L5" s="17">
-        <v>0.74939999999999996</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="M5" s="17">
-        <v>1241</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2858,22 +2871,22 @@
         <v>0.52610000000000001</v>
       </c>
       <c r="H6" s="17">
-        <v>0.7409</v>
+        <v>0.73329999999999995</v>
       </c>
       <c r="I6" s="17">
-        <v>1227</v>
+        <v>1026</v>
       </c>
       <c r="J6" s="17">
-        <v>0.74399999999999999</v>
+        <v>0.73619999999999997</v>
       </c>
       <c r="K6" s="17">
-        <v>1232</v>
+        <v>1030</v>
       </c>
       <c r="L6" s="17">
-        <v>0.74399999999999999</v>
+        <v>0.73619999999999997</v>
       </c>
       <c r="M6" s="17">
-        <v>1232</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2899,22 +2912,22 @@
         <v>0.51370000000000005</v>
       </c>
       <c r="H7" s="36">
-        <v>0.75790000000000002</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="I7" s="36">
-        <v>1255</v>
+        <v>1047</v>
       </c>
       <c r="J7" s="36">
-        <v>0.76029999999999998</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="K7" s="36">
-        <v>1259</v>
+        <v>1050</v>
       </c>
       <c r="L7" s="36">
-        <v>0.76029999999999998</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="M7" s="36">
-        <v>1259</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2940,22 +2953,22 @@
         <v>0.52449999999999997</v>
       </c>
       <c r="H8" s="35">
-        <v>0.74209999999999998</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="I8" s="35">
-        <v>1229</v>
+        <v>1047</v>
       </c>
       <c r="J8" s="35">
-        <v>0.74580000000000002</v>
+        <v>0.75129999999999997</v>
       </c>
       <c r="K8" s="35">
-        <v>1235</v>
+        <v>1051</v>
       </c>
       <c r="L8" s="35">
-        <v>0.74580000000000002</v>
+        <v>0.75129999999999997</v>
       </c>
       <c r="M8" s="35">
-        <v>1235</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2981,22 +2994,22 @@
         <v>0.52629999999999999</v>
       </c>
       <c r="H9" s="29">
-        <v>0.76329999999999998</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="I9" s="29">
-        <v>1264</v>
+        <v>1050</v>
       </c>
       <c r="J9" s="29">
-        <v>0.76629999999999998</v>
+        <v>0.75339999999999996</v>
       </c>
       <c r="K9" s="29">
-        <v>1269</v>
+        <v>1054</v>
       </c>
       <c r="L9" s="29">
-        <v>0.76629999999999998</v>
+        <v>0.75339999999999996</v>
       </c>
       <c r="M9" s="29">
-        <v>1269</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3022,22 +3035,22 @@
         <v>0.5131</v>
       </c>
       <c r="H10" s="5">
-        <v>0.77359999999999995</v>
+        <v>0.76480000000000004</v>
       </c>
       <c r="I10" s="5">
-        <v>1281</v>
+        <v>1070</v>
       </c>
       <c r="J10" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="K10" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
       <c r="L10" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="M10" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -3140,6 +3153,10 @@
       <c r="K15" s="76"/>
       <c r="L15" s="76"/>
       <c r="M15" s="77"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3172,7 +3189,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:M6"/>
+      <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3255,22 +3272,22 @@
         <v>0.46410000000000001</v>
       </c>
       <c r="H2" s="16">
-        <v>0.65939999999999999</v>
+        <v>0.66830000000000001</v>
       </c>
       <c r="I2" s="16">
-        <v>1092</v>
+        <v>935</v>
       </c>
       <c r="J2" s="16">
-        <v>0.66300000000000003</v>
+        <v>0.67120000000000002</v>
       </c>
       <c r="K2" s="16">
-        <v>1098</v>
+        <v>939</v>
       </c>
       <c r="L2" s="16">
-        <v>0.66300000000000003</v>
+        <v>0.67120000000000002</v>
       </c>
       <c r="M2" s="16">
-        <v>1098</v>
+        <v>939</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3296,22 +3313,22 @@
         <v>0.51090000000000002</v>
       </c>
       <c r="H3" s="26">
-        <v>0.72950000000000004</v>
+        <v>0.74119999999999997</v>
       </c>
       <c r="I3" s="26">
-        <v>1208</v>
+        <v>1037</v>
       </c>
       <c r="J3" s="26">
-        <v>0.73370000000000002</v>
+        <v>0.74339999999999995</v>
       </c>
       <c r="K3" s="26">
-        <v>1215</v>
+        <v>1040</v>
       </c>
       <c r="L3" s="26">
-        <v>0.73370000000000002</v>
+        <v>0.74339999999999995</v>
       </c>
       <c r="M3" s="26">
-        <v>1215</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -3337,22 +3354,22 @@
         <v>0.4773</v>
       </c>
       <c r="H4" s="26">
-        <v>0.69630000000000003</v>
+        <v>0.70189999999999997</v>
       </c>
       <c r="I4" s="26">
-        <v>1153</v>
+        <v>982</v>
       </c>
       <c r="J4" s="26">
-        <v>0.70050000000000001</v>
+        <v>0.70550000000000002</v>
       </c>
       <c r="K4" s="26">
-        <v>1160</v>
+        <v>987</v>
       </c>
       <c r="L4" s="26">
-        <v>0.70050000000000001</v>
+        <v>0.70550000000000002</v>
       </c>
       <c r="M4" s="26">
-        <v>1160</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -3378,22 +3395,22 @@
         <v>0.51570000000000005</v>
       </c>
       <c r="H5" s="26">
-        <v>0.72460000000000002</v>
+        <v>0.73050000000000004</v>
       </c>
       <c r="I5" s="26">
-        <v>1200</v>
+        <v>1022</v>
       </c>
       <c r="J5" s="26">
-        <v>0.7319</v>
+        <v>0.73340000000000005</v>
       </c>
       <c r="K5" s="26">
-        <v>1212</v>
+        <v>1026</v>
       </c>
       <c r="L5" s="26">
-        <v>0.7319</v>
+        <v>0.73340000000000005</v>
       </c>
       <c r="M5" s="26">
-        <v>1212</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3419,22 +3436,22 @@
         <v>0.51400000000000001</v>
       </c>
       <c r="H6" s="26">
-        <v>0.7198</v>
+        <v>0.71909999999999996</v>
       </c>
       <c r="I6" s="26">
-        <v>1192</v>
+        <v>1006</v>
       </c>
       <c r="J6" s="25">
-        <v>0.72399999999999998</v>
+        <v>0.72189999999999999</v>
       </c>
       <c r="K6" s="25">
-        <v>1199</v>
+        <v>1010</v>
       </c>
       <c r="L6" s="25">
-        <v>0.72399999999999998</v>
-      </c>
-      <c r="M6" s="26">
-        <v>1199</v>
+        <v>0.72189999999999999</v>
+      </c>
+      <c r="M6" s="25">
+        <v>1010</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3460,22 +3477,22 @@
         <v>0.50939999999999996</v>
       </c>
       <c r="H7" s="36">
-        <v>0.72709999999999997</v>
+        <v>0.72340000000000004</v>
       </c>
       <c r="I7" s="36">
-        <v>1204</v>
+        <v>1012</v>
       </c>
       <c r="J7" s="36">
-        <v>0.7319</v>
+        <v>0.72550000000000003</v>
       </c>
       <c r="K7" s="36">
-        <v>1212</v>
+        <v>1015</v>
       </c>
       <c r="L7" s="36">
-        <v>0.7319</v>
+        <v>0.72550000000000003</v>
       </c>
       <c r="M7" s="36">
-        <v>1212</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -3501,22 +3518,22 @@
         <v>0.51149999999999995</v>
       </c>
       <c r="H8" s="35">
-        <v>0.72519999999999996</v>
+        <v>0.74409999999999998</v>
       </c>
       <c r="I8" s="35">
-        <v>1201</v>
+        <v>1041</v>
       </c>
       <c r="J8" s="35">
-        <v>0.72950000000000004</v>
+        <v>0.747</v>
       </c>
       <c r="K8" s="35">
-        <v>1208</v>
+        <v>1045</v>
       </c>
       <c r="L8" s="35">
-        <v>0.72950000000000004</v>
+        <v>0.747</v>
       </c>
       <c r="M8" s="35">
-        <v>1208</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3542,22 +3559,22 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="H9" s="29">
-        <v>0.72040000000000004</v>
+        <v>0.72619999999999996</v>
       </c>
       <c r="I9" s="29">
-        <v>1193</v>
+        <v>1016</v>
       </c>
       <c r="J9" s="29">
-        <v>0.72399999999999998</v>
+        <v>0.72840000000000005</v>
       </c>
       <c r="K9" s="29">
-        <v>1199</v>
+        <v>1019</v>
       </c>
       <c r="L9" s="29">
-        <v>0.72399999999999998</v>
+        <v>0.72840000000000005</v>
       </c>
       <c r="M9" s="29">
-        <v>1199</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3583,22 +3600,22 @@
         <v>0.5131</v>
       </c>
       <c r="H10" s="5">
-        <v>0.77359999999999995</v>
+        <v>0.76480000000000004</v>
       </c>
       <c r="I10" s="5">
-        <v>1281</v>
+        <v>1070</v>
       </c>
       <c r="J10" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="K10" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
       <c r="L10" s="5">
-        <v>0.7772</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="M10" s="5">
-        <v>1287</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -3701,6 +3718,10 @@
       <c r="K15" s="76"/>
       <c r="L15" s="76"/>
       <c r="M15" s="77"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
@@ -3719,14 +3740,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -3955,6 +3968,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3965,23 +3986,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4000,6 +4004,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add learning signal precision data analysis
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1053" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFCDCC7E-EAC5-4CD5-A0A8-EBDAD967CE04}"/>
+  <xr:revisionPtr revIDLastSave="1152" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D903CE4-EC34-45EA-A265-E41C04CC1101}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2424" yWindow="0" windowWidth="20580" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
     <sheet name="opus_base Test" sheetId="2" r:id="rId2"/>
-    <sheet name="opus_big Validation + Test " sheetId="4" r:id="rId3"/>
-    <sheet name="M2M Validation + Test" sheetId="6" r:id="rId4"/>
+    <sheet name="opus_big Validation" sheetId="7" r:id="rId3"/>
+    <sheet name="opus_big Test " sheetId="4" r:id="rId4"/>
+    <sheet name="M2M (Deprecated)" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="63">
   <si>
     <t>Weight</t>
   </si>
@@ -209,9 +210,6 @@
     <t>WCE with unsampled training data and glossary, weight 1.25</t>
   </si>
   <si>
-    <t>Adaptive WCE</t>
-  </si>
-  <si>
     <t>Bands = 6, upper bound weight = 1.25, band interval = 0.05</t>
   </si>
   <si>
@@ -224,13 +222,13 @@
     <t>Bands = 6, upper bound weight = 1.5, band interval = 0.1, 0.25 sampled glossary</t>
   </si>
   <si>
-    <t>Runtime</t>
-  </si>
-  <si>
     <t>Correct Predictions</t>
   </si>
   <si>
     <t>M2M100_418M</t>
+  </si>
+  <si>
+    <t>Choi et al. (2022)</t>
   </si>
 </sst>
 </file>
@@ -238,7 +236,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -304,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -577,11 +575,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,50 +697,134 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,18 +838,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,57 +850,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,11 +886,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1102,10 +1182,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L48"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1199,7 @@
     <col min="8" max="8" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1142,14 +1223,14 @@
       </c>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="65">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1174,10 +1255,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="67"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1193,17 +1274,17 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3">
-        <f>MEDIAN(E18:E29)</f>
+        <f>MEDIAN(E22:E33)</f>
         <v>42.64105</v>
       </c>
       <c r="J3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="67"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1219,10 +1300,10 @@
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="67"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1238,10 +1319,10 @@
       </c>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1259,10 +1340,10 @@
       </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="67"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1278,10 +1359,10 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="67"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1297,10 +1378,10 @@
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="67"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1316,10 +1397,10 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="67"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1332,15 +1413,15 @@
         <v>11230.0195</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" ref="G10:G17" si="1">F10*32.6*0.3 / 1000</f>
+        <f t="shared" ref="G10:G21" si="1">F10*32.6*0.3 / 1000</f>
         <v>109.82959071000001</v>
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="67"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1356,10 +1437,10 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="67"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1375,10 +1456,10 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="67"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1393,17 +1474,11 @@
         <v>201.28675508399999</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="67"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1420,20 +1495,11 @@
         <v>101.14486073400001</v>
       </c>
       <c r="H14" s="10"/>
-      <c r="I14">
-        <v>42.688000000000002</v>
-      </c>
-      <c r="J14">
-        <v>25883.389200000001</v>
-      </c>
-      <c r="L14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="67"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1449,10 +1515,10 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="67"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1469,9 +1535,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1488,540 +1554,619 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="46">
-        <v>0.75</v>
-      </c>
-      <c r="C18" s="46"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="63">
+        <v>1</v>
+      </c>
+      <c r="C18" s="71"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
       <c r="E18" s="19">
-        <v>42.6248</v>
-      </c>
-      <c r="F18" s="7">
-        <v>15649.238600000001</v>
+        <v>42.660200000000003</v>
+      </c>
+      <c r="F18" s="26">
+        <v>15173.948</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" ref="G18:G42" si="2">F18*32.6*0.3 / 1000</f>
-        <v>153.049553508</v>
+        <f t="shared" si="1"/>
+        <v>148.40121144</v>
       </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
       <c r="E19" s="19">
-        <v>42.568800000000003</v>
-      </c>
-      <c r="F19" s="7">
-        <v>15634.0206</v>
+        <v>42.821899999999999</v>
+      </c>
+      <c r="F19" s="26">
+        <v>20850.177599999999</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="2"/>
-        <v>152.900721468</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>203.91473692799997</v>
+      </c>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
       <c r="E20" s="19">
-        <v>42.657299999999999</v>
-      </c>
-      <c r="F20" s="7">
-        <v>24736.3887</v>
+        <v>42.5351</v>
+      </c>
+      <c r="F20" s="26">
+        <v>20964.995299999999</v>
       </c>
       <c r="G20" s="7">
-        <f t="shared" si="2"/>
-        <v>241.92188148599999</v>
+        <f t="shared" si="1"/>
+        <v>205.03765403400001</v>
       </c>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="19">
-        <v>42.586300000000001</v>
-      </c>
-      <c r="F21" s="7">
-        <v>25533.498100000001</v>
+        <v>42.761600000000001</v>
+      </c>
+      <c r="F21" s="26">
+        <v>24527.117200000001</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="2"/>
-        <v>249.71761141800002</v>
+        <f t="shared" si="1"/>
+        <v>239.87520621599998</v>
       </c>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="C22" s="46"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="71"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
       <c r="E22" s="19">
-        <v>42.834800000000001</v>
-      </c>
-      <c r="F22" s="7">
-        <v>22345.029500000001</v>
+        <v>42.6248</v>
+      </c>
+      <c r="F22" s="26">
+        <v>18188.4378</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="2"/>
-        <v>218.53438851000001</v>
+        <f t="shared" ref="G22:G46" si="2">F22*32.6*0.3 / 1000</f>
+        <v>177.88292168399997</v>
       </c>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
       <c r="E23" s="19">
-        <v>42.8322</v>
-      </c>
-      <c r="F23" s="7">
-        <v>25586.411599999999</v>
+        <v>42.568800000000003</v>
+      </c>
+      <c r="F23" s="26">
+        <v>15068.799300000001</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="2"/>
-        <v>250.23510544799998</v>
-      </c>
-      <c r="H23" s="10"/>
+        <v>147.372857154</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
       <c r="E24" s="19">
-        <v>42.7468</v>
-      </c>
-      <c r="F24" s="7">
-        <v>25118.774000000001</v>
+        <v>42.657299999999999</v>
+      </c>
+      <c r="F24" s="26">
+        <v>25092.556199999999</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="2"/>
-        <v>245.66160972</v>
+        <v>245.40519963599999</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="19">
-        <v>42.115699999999997</v>
-      </c>
-      <c r="F25" s="7">
-        <v>15740.974700000001</v>
+        <v>42.586300000000001</v>
+      </c>
+      <c r="F25" s="26">
+        <v>25398.764299999999</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="2"/>
-        <v>153.94673256600001</v>
+        <v>248.39991485399997</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
-      <c r="B26" s="46">
-        <v>0.25</v>
-      </c>
-      <c r="C26" s="46"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="71"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
       <c r="E26" s="19">
-        <v>42.577399999999997</v>
-      </c>
-      <c r="F26" s="7">
-        <v>15012.536</v>
+        <v>42.834800000000001</v>
+      </c>
+      <c r="F26" s="26">
+        <v>25998.02</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="2"/>
-        <v>146.82260208000002</v>
+        <v>254.2606356</v>
       </c>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
-      <c r="E27" s="23">
-        <v>42.997799999999998</v>
-      </c>
-      <c r="F27" s="7">
-        <v>24740.625</v>
+      <c r="E27" s="19">
+        <v>42.8322</v>
+      </c>
+      <c r="F27" s="26">
+        <v>25586.411599999999</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" si="2"/>
-        <v>241.9633125</v>
+        <v>250.23510544799998</v>
       </c>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
       <c r="E28" s="19">
-        <v>42.590800000000002</v>
-      </c>
-      <c r="F28" s="7">
-        <v>24592.9486</v>
+        <v>42.7468</v>
+      </c>
+      <c r="F28" s="26">
+        <v>28975.652399999999</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="2"/>
-        <v>240.51903730800001</v>
+        <v>283.38188047199998</v>
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="67"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="6">
         <v>2</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="19">
+        <v>42.115699999999997</v>
+      </c>
+      <c r="F29" s="26">
+        <v>15740.974700000001</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="2"/>
+        <v>153.94673256600001</v>
+      </c>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="67"/>
+      <c r="B30" s="71">
+        <v>0.25</v>
+      </c>
+      <c r="C30" s="71"/>
+      <c r="D30" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E30" s="19">
+        <v>42.577399999999997</v>
+      </c>
+      <c r="F30" s="26">
+        <v>15201.500099999999</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="2"/>
+        <v>148.67067097799998</v>
+      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="67"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E31" s="43">
+        <v>42.997799999999998</v>
+      </c>
+      <c r="F31" s="26">
+        <v>25395.683000000001</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="2"/>
+        <v>248.36977973999998</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="67"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E32" s="19">
+        <v>42.590800000000002</v>
+      </c>
+      <c r="F32" s="26">
+        <v>24988.770499999999</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="2"/>
+        <v>244.39017548999999</v>
+      </c>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="68"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="8">
+        <v>2</v>
+      </c>
+      <c r="E33" s="21">
         <v>42.779699999999998</v>
       </c>
-      <c r="F29" s="9">
-        <v>24985.3393</v>
-      </c>
-      <c r="G29" s="9">
+      <c r="F33" s="27">
+        <v>25648.176599999999</v>
+      </c>
+      <c r="G33" s="9">
         <f t="shared" si="2"/>
-        <v>244.35661835400001</v>
-      </c>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="41" t="s">
+        <v>250.83916714799997</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B34" s="73">
         <v>0.1</v>
       </c>
-      <c r="C30" s="48">
+      <c r="C34" s="73">
         <v>1</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D34" s="4">
         <v>1.25</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E34" s="22">
         <v>43.001100000000001</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F34" s="5">
         <v>25190.439699999999</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G34" s="5">
         <f t="shared" si="2"/>
         <v>246.36250026599998</v>
       </c>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="6">
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="6">
         <v>1.5</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E35" s="19">
         <v>42.782299999999999</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F35" s="7">
         <v>20479.9146</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G35" s="7">
         <f t="shared" si="2"/>
         <v>200.29356478800003</v>
       </c>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="6">
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="6">
         <v>1.75</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E36" s="19">
         <v>42.821300000000001</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F36" s="7">
         <v>25430.924900000002</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G36" s="7">
         <f t="shared" si="2"/>
         <v>248.71444552200003</v>
       </c>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="43"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="8">
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="48"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="8">
         <v>2</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E37" s="21">
         <v>41.998399999999997</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F37" s="9">
         <v>15306.2101</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G37" s="9">
         <f t="shared" si="2"/>
         <v>149.69473477800003</v>
       </c>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="49" t="s">
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B38" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="4">
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F38" s="5">
         <v>12104.798500000001</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G38" s="5">
         <f t="shared" si="2"/>
         <v>118.38492933000002</v>
       </c>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43"/>
-      <c r="B35" s="50" t="s">
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="48"/>
+      <c r="B39" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="15">
+      <c r="C39" s="51"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="15">
         <v>42.128999999999998</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F39" s="9">
         <v>9021.1026999999995</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G39" s="9">
         <f t="shared" si="2"/>
         <v>88.226384405999994</v>
       </c>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="49" t="s">
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B40" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="4" t="s">
+      <c r="C40" s="61"/>
+      <c r="D40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E40" s="4">
         <v>41.673900000000003</v>
       </c>
-      <c r="F36" s="5">
-        <f>F42 + 815.0048</f>
+      <c r="F40" s="5">
+        <f>F46 + 815.0048</f>
         <v>18004.647499999999</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G40" s="5">
         <f t="shared" si="2"/>
         <v>176.08545254999999</v>
       </c>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="6" t="s">
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="49"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E41" s="6">
         <v>38.872199999999999</v>
       </c>
-      <c r="F37" s="7">
-        <f>F42 + 1547.1448</f>
+      <c r="F41" s="7">
+        <f>F46 + 1547.1448</f>
         <v>18736.787499999999</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G41" s="7">
         <f t="shared" si="2"/>
         <v>183.24578174999999</v>
       </c>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="59" t="s">
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="49"/>
+      <c r="B42" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="60"/>
-      <c r="D38" s="6" t="s">
+      <c r="C42" s="57"/>
+      <c r="D42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E42" s="13">
         <v>41.738300000000002</v>
       </c>
-      <c r="F38" s="7">
-        <f>F42 + 859.7958</f>
+      <c r="F42" s="7">
+        <f>F46 + 859.7958</f>
         <v>18049.4385</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G42" s="7">
         <f t="shared" si="2"/>
         <v>176.52350852999999</v>
       </c>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="1:12" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="43"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="8" t="s">
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="48"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E43" s="8">
         <v>40.942300000000003</v>
       </c>
-      <c r="F39" s="9">
-        <f>F42 + 1529.7841</f>
+      <c r="F43" s="9">
+        <f>F46 + 1529.7841</f>
         <v>18719.426800000001</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G43" s="9">
         <f t="shared" si="2"/>
         <v>183.07599410400002</v>
       </c>
-      <c r="H39" s="10"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="49" t="s">
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B44" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="4">
+      <c r="C44" s="45"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F44" s="5">
         <v>13749.5393</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G44" s="5">
         <f t="shared" si="2"/>
         <v>134.47049435399998</v>
       </c>
-      <c r="H40" s="10"/>
-    </row>
-    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="43"/>
-      <c r="B41" s="50" t="s">
+      <c r="H44" s="10"/>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="48"/>
+      <c r="B45" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="15">
+      <c r="C45" s="51"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="15">
         <v>42.606000000000002</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F45" s="9">
         <v>8859.1144999999997</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G45" s="9">
         <f t="shared" si="2"/>
         <v>86.642139810000003</v>
       </c>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="44" t="s">
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="5">
+      <c r="B46" s="70"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="5">
         <v>42.67</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F46" s="5">
         <v>17189.6427</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G46" s="5">
         <f t="shared" si="2"/>
         <v>168.114705606</v>
       </c>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L48" s="12"/>
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="52" spans="12:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L52" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="A2:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A42:D42"/>
+  <mergeCells count="23">
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A2:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A46:D46"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C29"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C14:C33"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2030,10 +2175,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
-  <dimension ref="A1:M18"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2078,19 +2224,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2115,22 +2261,22 @@
       <c r="G2" s="16">
         <v>0.48980000000000001</v>
       </c>
-      <c r="H2" s="78">
+      <c r="H2" s="35">
         <v>0.72270000000000001</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="24">
         <v>1011</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="24">
         <v>0.72550000000000003</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="24">
         <v>1015</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="24">
         <v>0.72550000000000003</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="24">
         <v>1015</v>
       </c>
     </row>
@@ -2156,22 +2302,22 @@
       <c r="G3" s="17">
         <v>0.4894</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <v>0.68620000000000003</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <v>960</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="25">
         <v>0.68910000000000005</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <v>964</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="25">
         <v>0.74550000000000005</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="25">
         <v>1043</v>
       </c>
     </row>
@@ -2197,22 +2343,22 @@
       <c r="G4" s="17">
         <v>0.4723</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="26">
         <v>0.67410000000000003</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="26">
         <v>943</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="26">
         <v>0.67759999999999998</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="26">
         <v>948</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="26">
         <v>0.74409999999999998</v>
       </c>
-      <c r="M4" s="27">
+      <c r="M4" s="26">
         <v>1041</v>
       </c>
     </row>
@@ -2238,22 +2384,22 @@
       <c r="G5" s="17">
         <v>0.4834</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <v>0.67479999999999996</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="26">
         <v>944</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="26">
         <v>0.67759999999999998</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
         <v>948</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="26">
         <v>0.74339999999999995</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="26">
         <v>1040</v>
       </c>
     </row>
@@ -2279,22 +2425,22 @@
       <c r="G6" s="17">
         <v>0.49020000000000002</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <v>0.67479999999999996</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="26">
         <v>944</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="26">
         <v>0.67689999999999995</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="26">
         <v>947</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="26">
         <v>0.73480000000000001</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="26">
         <v>1028</v>
       </c>
     </row>
@@ -2308,311 +2454,270 @@
       <c r="C7" s="21">
         <v>43.001100000000001</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="33">
         <v>33.6</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>52.72</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <v>69.66</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="33">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>0.6905</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="27">
         <v>966</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="27">
         <v>0.69410000000000005</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="27">
         <v>971</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
         <v>0.75270000000000004</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="27">
         <v>1053</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="31">
         <v>42.997799999999998</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="32">
         <v>33.450000000000003</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="32">
         <v>52.55</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="32">
         <v>69.88</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="32">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="32">
         <v>0.68620000000000003</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="32">
         <v>960</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="32">
         <v>0.68979999999999997</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="32">
         <v>965</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="32">
         <v>0.74770000000000003</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="32">
         <v>1046</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="33">
-        <v>42.688000000000002</v>
-      </c>
-      <c r="D9" s="33">
-        <v>33.4</v>
-      </c>
-      <c r="E9" s="33">
-        <v>52.61</v>
-      </c>
-      <c r="F9" s="33">
-        <v>69.459999999999994</v>
-      </c>
-      <c r="G9" s="33">
-        <v>0.48449999999999999</v>
-      </c>
-      <c r="H9" s="33">
-        <v>0.68189999999999995</v>
-      </c>
-      <c r="I9" s="33">
-        <v>954</v>
-      </c>
-      <c r="J9" s="33">
-        <v>0.6855</v>
-      </c>
-      <c r="K9" s="33">
-        <v>959</v>
-      </c>
-      <c r="L9" s="33">
+      <c r="B9" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="30">
+        <v>42.839799999999997</v>
+      </c>
+      <c r="D9" s="29">
+        <v>34.11</v>
+      </c>
+      <c r="E9" s="29">
+        <v>53.06</v>
+      </c>
+      <c r="F9" s="29">
+        <v>68.42</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0.4894</v>
+      </c>
+      <c r="H9" s="29">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="I9" s="29">
+        <v>958</v>
+      </c>
+      <c r="J9" s="29">
+        <v>0.68759999999999999</v>
+      </c>
+      <c r="K9" s="29">
+        <v>962</v>
+      </c>
+      <c r="L9" s="29">
         <v>0.74480000000000002</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="29">
         <v>1042</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="32">
-        <v>42.839799999999997</v>
-      </c>
-      <c r="D10" s="31">
-        <v>34.11</v>
-      </c>
-      <c r="E10" s="31">
-        <v>53.06</v>
-      </c>
-      <c r="F10" s="31">
-        <v>68.42</v>
-      </c>
-      <c r="G10" s="31">
-        <v>0.4894</v>
-      </c>
-      <c r="H10" s="31">
-        <v>0.68479999999999996</v>
-      </c>
-      <c r="I10" s="31">
-        <v>958</v>
-      </c>
-      <c r="J10" s="31">
-        <v>0.68759999999999999</v>
-      </c>
-      <c r="K10" s="31">
-        <v>962</v>
-      </c>
-      <c r="L10" s="31">
-        <v>0.74480000000000002</v>
-      </c>
-      <c r="M10" s="31">
-        <v>1042</v>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5">
+        <v>37.71</v>
+      </c>
+      <c r="E10" s="5">
+        <v>55.04</v>
+      </c>
+      <c r="F10" s="5">
+        <v>66.48</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.5131</v>
+      </c>
+      <c r="H10" s="36">
+        <v>0.76480000000000004</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1070</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1073</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1073</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="5">
-        <v>37.71</v>
-      </c>
-      <c r="E11" s="5">
-        <v>55.04</v>
-      </c>
-      <c r="F11" s="5">
-        <v>66.48</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.5131</v>
-      </c>
-      <c r="H11" s="79">
-        <v>0.76480000000000004</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1070</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="K11" s="5">
-        <v>1073</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="M11" s="5">
-        <v>1073</v>
-      </c>
+      <c r="A11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="7">
+        <v>36.130000000000003</v>
+      </c>
+      <c r="E11" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="79"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="67"/>
+        <v>42</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="75"/>
       <c r="D12" s="7">
-        <v>36.130000000000003</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="71"/>
+        <v>35.5</v>
+      </c>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="67"/>
+        <v>43</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="7">
-        <v>35.5</v>
-      </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="74"/>
+        <v>35.409999999999997</v>
+      </c>
+      <c r="E13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
+        <v>44</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="7">
-        <v>35.409999999999997</v>
-      </c>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="74"/>
+        <v>35.18</v>
+      </c>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
+        <v>45</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="7">
-        <v>35.18</v>
-      </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="74"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="7">
         <v>31.63</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="77"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="E12:M16"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="E11:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2620,11 +2725,786 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408B2997-0DD0-4206-AAF3-1F52C502CA37}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:L47"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="6" width="26.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="65">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
+        <f t="shared" ref="G2:G41" si="0">F2*32.6*0.3 / 1000</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" t="e">
+        <f>MEDIAN(E2:E13)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="67"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" t="e">
+        <f>MEDIAN(E22:E33)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="67"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="67"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="67"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="67"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="67"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="67"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="67"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="67"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="67"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="67"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E14" s="20">
+        <v>43.406100000000002</v>
+      </c>
+      <c r="F14" s="7">
+        <v>21021.619699999999</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>205.59144066599998</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="67"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="19">
+        <v>42.881100000000004</v>
+      </c>
+      <c r="F15" s="7">
+        <v>14726.3397</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>144.02360226600001</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="67"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E16" s="19">
+        <v>43.041400000000003</v>
+      </c>
+      <c r="F16" s="7">
+        <v>20828.407899999998</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>203.70182926199999</v>
+      </c>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="67"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="19">
+        <v>42.716700000000003</v>
+      </c>
+      <c r="F17" s="7">
+        <v>14642.5874</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>143.20450477199998</v>
+      </c>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="67"/>
+      <c r="B18" s="63">
+        <v>1</v>
+      </c>
+      <c r="C18" s="71"/>
+      <c r="D18" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="67"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="67"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="67"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="6">
+        <v>2</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="67"/>
+      <c r="B22" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="71"/>
+      <c r="D22" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="67"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="67"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="67"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="6">
+        <v>2</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="67"/>
+      <c r="B26" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="71"/>
+      <c r="D26" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="67"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="67"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="67"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="67"/>
+      <c r="B30" s="71">
+        <v>0.25</v>
+      </c>
+      <c r="C30" s="71"/>
+      <c r="D30" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="67"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="67"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="68"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="8">
+        <v>2</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="C34" s="73">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="E34" s="22">
+        <v>43.105200000000004</v>
+      </c>
+      <c r="F34" s="5">
+        <v>22497.546399999999</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="0"/>
+        <v>220.02600379199998</v>
+      </c>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E35" s="19">
+        <v>42.871299999999998</v>
+      </c>
+      <c r="F35" s="7">
+        <v>16458.1312</v>
+      </c>
+      <c r="G35" s="7">
+        <f t="shared" si="0"/>
+        <v>160.96052313600001</v>
+      </c>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="E36" s="19">
+        <v>43.089599999999997</v>
+      </c>
+      <c r="F36" s="7">
+        <v>28476.754099999998</v>
+      </c>
+      <c r="G36" s="7">
+        <f t="shared" si="0"/>
+        <v>278.50265509799993</v>
+      </c>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="48"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="8">
+        <v>2</v>
+      </c>
+      <c r="E37" s="21">
+        <v>42.917099999999998</v>
+      </c>
+      <c r="F37" s="9">
+        <v>15470.588400000001</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="0"/>
+        <v>151.302354552</v>
+      </c>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="8">
+        <v>43.123899999999999</v>
+      </c>
+      <c r="F38" s="9">
+        <v>17977.4303</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="0"/>
+        <v>175.81926833400001</v>
+      </c>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="87"/>
+      <c r="D39" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="40">
+        <v>42.252800000000001</v>
+      </c>
+      <c r="F39" s="41">
+        <v>1125.7265</v>
+      </c>
+      <c r="G39" s="41">
+        <f t="shared" si="0"/>
+        <v>11.00960517</v>
+      </c>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="88"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="42">
+        <v>43.224200000000003</v>
+      </c>
+      <c r="F40" s="38">
+        <v>12175.0232</v>
+      </c>
+      <c r="G40" s="38">
+        <f t="shared" si="0"/>
+        <v>119.07172689599999</v>
+      </c>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="70"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="5">
+        <v>42.909700000000001</v>
+      </c>
+      <c r="F41" s="5">
+        <v>16676.394700000001</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="0"/>
+        <v>163.09514016599999</v>
+      </c>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L47" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="A2:A33"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2669,19 +3549,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2899,116 +3779,116 @@
       <c r="C7" s="9">
         <v>43.105200000000004</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="33">
         <v>33.86</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>53.03</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <v>68.69</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="33">
         <v>0.51370000000000005</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="33">
         <v>0.74839999999999995</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="33">
         <v>1047</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="33">
         <v>0.75049999999999994</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="33">
         <v>1050</v>
       </c>
-      <c r="L7" s="36">
+      <c r="L7" s="33">
         <v>0.75049999999999994</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="33">
         <v>1050</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="31">
         <v>43.406100000000002</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="32">
         <v>33.82</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="32">
         <v>53.02</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="32">
         <v>68.540000000000006</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="32">
         <v>0.52449999999999997</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="32">
         <v>0.74839999999999995</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="32">
         <v>1047</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="32">
         <v>0.75129999999999997</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="32">
         <v>1051</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="32">
         <v>0.75129999999999997</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="32">
         <v>1051</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="37">
+      <c r="B9" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="34">
         <v>43.305199999999999</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>34.299999999999997</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>53.32</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>67.87</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="28">
         <v>0.52629999999999999</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="28">
         <v>0.75049999999999994</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="28">
         <v>1050</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="28">
         <v>0.75339999999999996</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="28">
         <v>1054</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="28">
         <v>0.75339999999999996</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="28">
         <v>1054</v>
       </c>
     </row>
@@ -3019,7 +3899,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="75" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3060,108 +3940,108 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="71"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="79"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="74"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="74"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="74"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="68"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="77"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -3184,8 +4064,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AE9F30-CD4B-42DC-84E4-E64EA556D182}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3234,19 +4115,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -3254,7 +4135,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>52</v>
@@ -3300,34 +4181,34 @@
       <c r="C3" s="7">
         <v>40.444299999999998</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>32.83</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>52</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>69.88</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>0.51090000000000002</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <v>0.74119999999999997</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <v>1037</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="25">
         <v>0.74339999999999995</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <v>1040</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="25">
         <v>0.74339999999999995</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="25">
         <v>1040</v>
       </c>
     </row>
@@ -3341,34 +4222,34 @@
       <c r="C4" s="7">
         <v>38.722200000000001</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>31.47</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="25">
         <v>50.74</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>71.33</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>0.4773</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <v>0.70189999999999997</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <v>982</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>0.70550000000000002</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <v>987</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="25">
         <v>0.70550000000000002</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="25">
         <v>987</v>
       </c>
     </row>
@@ -3382,34 +4263,34 @@
       <c r="C5" s="7">
         <v>40.642400000000002</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>32.68</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>51.81</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>69.739999999999995</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0.51570000000000005</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>0.73050000000000004</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <v>1022</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <v>0.73340000000000005</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <v>1026</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="25">
         <v>0.73340000000000005</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="25">
         <v>1026</v>
       </c>
     </row>
@@ -3420,37 +4301,37 @@
       <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>40.634</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>33.090000000000003</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>51.98</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>69.52</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>0.51400000000000001</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>0.71909999999999996</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>1006</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="24">
         <v>0.72189999999999999</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="24">
         <v>1010</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="24">
         <v>0.72189999999999999</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="24">
         <v>1010</v>
       </c>
     </row>
@@ -3464,116 +4345,116 @@
       <c r="C7" s="9">
         <v>40.878</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="33">
         <v>32.130000000000003</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>51.44</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <v>70.7</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="33">
         <v>0.50939999999999996</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="33">
         <v>0.72340000000000004</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="33">
         <v>1012</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="33">
         <v>0.72550000000000003</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="33">
         <v>1015</v>
       </c>
-      <c r="L7" s="36">
+      <c r="L7" s="33">
         <v>0.72550000000000003</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="33">
         <v>1015</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="31">
         <v>40.930199999999999</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="32">
         <v>33.03</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="32">
         <v>52.01</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="32">
         <v>70.040000000000006</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="32">
         <v>0.51149999999999995</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="32">
         <v>0.74409999999999998</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="32">
         <v>1041</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="32">
         <v>0.747</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="32">
         <v>1045</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="32">
         <v>0.747</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="32">
         <v>1045</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="37">
+      <c r="B9" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="34">
         <v>40.607199999999999</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>31.77</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>51.23</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>70.650000000000006</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="28">
         <v>0.50800000000000001</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="28">
         <v>0.72619999999999996</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="28">
         <v>1016</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="28">
         <v>0.72840000000000005</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="28">
         <v>1019</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="28">
         <v>0.72840000000000005</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="28">
         <v>1019</v>
       </c>
     </row>
@@ -3584,7 +4465,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="75" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -3625,108 +4506,108 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="71"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="79"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="74"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="74"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="74"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="68"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="77"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3740,6 +4621,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -3968,14 +4857,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3986,6 +4867,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4004,23 +4902,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update opus-big wce hyperparameter search
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1152" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D903CE4-EC34-45EA-A265-E41C04CC1101}"/>
+  <xr:revisionPtr revIDLastSave="1260" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D74945AD-970F-4123-AD68-659996C585F1}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="0" windowWidth="20580" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="70">
   <si>
     <t>Weight</t>
   </si>
@@ -204,9 +204,6 @@
     <t>OPUS-MT-TC-BIG-EN-FR</t>
   </si>
   <si>
-    <t>WCE using best hyperparameters</t>
-  </si>
-  <si>
     <t>WCE with unsampled training data and glossary, weight 1.25</t>
   </si>
   <si>
@@ -216,12 +213,6 @@
     <t>Baseline + Adaptive WCE</t>
   </si>
   <si>
-    <t>Baseline + Adaptive WCE (Best Hyp)</t>
-  </si>
-  <si>
-    <t>Bands = 6, upper bound weight = 1.5, band interval = 0.1, 0.25 sampled glossary</t>
-  </si>
-  <si>
     <t>Correct Predictions</t>
   </si>
   <si>
@@ -229,6 +220,36 @@
   </si>
   <si>
     <t>Choi et al. (2022)</t>
+  </si>
+  <si>
+    <t>Ailem-Adapted</t>
+  </si>
+  <si>
+    <t>Ailem-Antagonistic</t>
+  </si>
+  <si>
+    <t>WCE-Adapted</t>
+  </si>
+  <si>
+    <t>WCE-Antagonistic</t>
+  </si>
+  <si>
+    <t>Ailem-Random</t>
+  </si>
+  <si>
+    <t>WCE-Random</t>
+  </si>
+  <si>
+    <t>0.75 train sample, full glossary, weight 1.25</t>
+  </si>
+  <si>
+    <t>0.1 train sample, full glossary, weight 1.25</t>
+  </si>
+  <si>
+    <t>0.25 train sample, full glossary, weight 1.5</t>
+  </si>
+  <si>
+    <t>0.25 train sample, full glossary, upper weight 1.5, bands 6</t>
   </si>
 </sst>
 </file>
@@ -631,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,6 +781,84 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,24 +868,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -815,39 +896,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1185,7 +1233,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -1224,13 +1272,13 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="65">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1256,9 +1304,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1282,9 +1330,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1301,9 +1349,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1320,9 +1368,9 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="67"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71">
+      <c r="A6" s="57"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1341,9 +1389,9 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1360,9 +1408,9 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1379,9 +1427,9 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1398,9 +1446,9 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71">
+      <c r="A10" s="57"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1419,9 +1467,9 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1438,9 +1486,9 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1457,9 +1505,9 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1476,9 +1524,9 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71">
+      <c r="A14" s="57"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1497,9 +1545,9 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1516,9 +1564,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1535,9 +1583,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1554,11 +1602,11 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
-      <c r="B18" s="63">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="71"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1575,9 +1623,9 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="71"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1642,9 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="71"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1613,9 +1661,9 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="71"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1632,11 +1680,11 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="71">
+      <c r="A22" s="57"/>
+      <c r="B22" s="63">
         <v>0.75</v>
       </c>
-      <c r="C22" s="71"/>
+      <c r="C22" s="63"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1653,9 +1701,9 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1671,9 +1719,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1690,9 +1738,9 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1709,11 +1757,11 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="71">
+      <c r="A26" s="57"/>
+      <c r="B26" s="63">
         <v>0.5</v>
       </c>
-      <c r="C26" s="71"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1730,9 +1778,9 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1749,9 +1797,9 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1768,9 +1816,9 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1787,11 +1835,11 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="67"/>
-      <c r="B30" s="71">
+      <c r="A30" s="57"/>
+      <c r="B30" s="63">
         <v>0.25</v>
       </c>
-      <c r="C30" s="71"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1808,9 +1856,9 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1827,9 +1875,9 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1846,9 +1894,9 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="68"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1865,13 +1913,13 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="73">
+      <c r="B34" s="65">
         <v>0.1</v>
       </c>
-      <c r="C34" s="73">
+      <c r="C34" s="65">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1890,9 +1938,9 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="49"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1909,9 +1957,9 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="49"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1928,9 +1976,9 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="48"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1947,14 +1995,14 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="55"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1968,12 +2016,12 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="48"/>
-      <c r="B39" s="50" t="s">
+      <c r="A39" s="61"/>
+      <c r="B39" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="15">
         <v>42.128999999999998</v>
       </c>
@@ -1987,13 +2035,13 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="61"/>
+      <c r="C40" s="81"/>
       <c r="D40" s="4" t="s">
         <v>16</v>
       </c>
@@ -2011,9 +2059,9 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="49"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="62"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="82"/>
       <c r="D41" s="6" t="s">
         <v>15</v>
       </c>
@@ -2031,11 +2079,11 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="49"/>
-      <c r="B42" s="56" t="s">
+      <c r="A42" s="60"/>
+      <c r="B42" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="57"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="6" t="s">
         <v>16</v>
       </c>
@@ -2053,9 +2101,9 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="48"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="59"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79"/>
       <c r="D43" s="8" t="s">
         <v>15</v>
       </c>
@@ -2073,14 +2121,14 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="45"/>
-      <c r="D44" s="46"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -2094,12 +2142,12 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="48"/>
-      <c r="B45" s="50" t="s">
+      <c r="A45" s="61"/>
+      <c r="B45" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="15">
         <v>42.606000000000002</v>
       </c>
@@ -2113,12 +2161,12 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="70" t="s">
+      <c r="A46" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2144,6 +2192,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2160,13 +2215,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2176,10 +2224,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8347FF-D187-4D6C-9C41-B96FB5C52911}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2224,19 +2272,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2403,321 +2451,406 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>42.606000000000002</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="45">
         <v>33.090000000000003</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="45">
         <v>52.29</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="45">
         <v>69.459999999999994</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="45">
         <v>0.49020000000000002</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="27">
         <v>0.67479999999999996</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="27">
         <v>944</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="27">
         <v>0.67689999999999995</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="27">
         <v>947</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="27">
         <v>0.73480000000000001</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="27">
         <v>1028</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="21">
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="18">
         <v>43.001100000000001</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="24">
         <v>33.6</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="24">
         <v>52.72</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="24">
         <v>69.66</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="24">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="49">
         <v>0.6905</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="49">
         <v>966</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="49">
         <v>0.69410000000000005</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="49">
         <v>971</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="49">
         <v>0.75270000000000004</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7" s="49">
         <v>1053</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="31">
+      <c r="B11" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="31">
         <v>42.997799999999998</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D11" s="32">
         <v>33.450000000000003</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E11" s="32">
         <v>52.55</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F11" s="32">
         <v>69.88</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G11" s="32">
         <v>0.48559999999999998</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H11" s="32">
         <v>0.68620000000000003</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I11" s="32">
         <v>960</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J11" s="32">
         <v>0.68979999999999997</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K11" s="32">
         <v>965</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L11" s="32">
         <v>0.74770000000000003</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M11" s="32">
         <v>1046</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="30">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="51">
         <v>42.839799999999997</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D12" s="50">
         <v>34.11</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E12" s="50">
         <v>53.06</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F12" s="50">
         <v>68.42</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G12" s="50">
         <v>0.4894</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H12" s="50">
         <v>0.68479999999999996</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I12" s="50">
         <v>958</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J12" s="50">
         <v>0.68759999999999999</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K12" s="50">
         <v>962</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L12" s="50">
         <v>0.74480000000000002</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M12" s="50">
         <v>1042</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C15" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D15" s="5">
         <v>37.71</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E15" s="5">
         <v>55.04</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F15" s="5">
         <v>66.48</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G15" s="5">
         <v>0.5131</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H15" s="36">
         <v>0.76480000000000004</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I15" s="5">
         <v>1070</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J15" s="5">
         <v>0.76700000000000002</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K15" s="5">
         <v>1073</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L15" s="5">
         <v>0.76700000000000002</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M15" s="5">
         <v>1073</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="7">
+      <c r="C16" s="84"/>
+      <c r="D16" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E16" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="79"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="88"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B17" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="7">
+      <c r="C17" s="84"/>
+      <c r="D17" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="82"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="E17" s="89"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="91"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="7">
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="80"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="91"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="7">
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="E19" s="89"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="91"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="7">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="85"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="94"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="E11:M15"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="E16:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2729,8 +2862,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2768,213 +2901,261 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="65">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
         <v>1.25</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="18">
+        <v>43.375500000000002</v>
+      </c>
+      <c r="F2" s="5">
+        <v>28644.873200000002</v>
+      </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G41" si="0">F2*32.6*0.3 / 1000</f>
-        <v>0</v>
+        <v>280.14685989600002</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" t="e">
+      <c r="I2">
         <f>MEDIAN(E2:E13)</f>
-        <v>#NUM!</v>
+        <v>43.011849999999995</v>
       </c>
       <c r="J2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="19">
+        <v>43.087299999999999</v>
+      </c>
+      <c r="F3" s="7">
+        <v>28898.543900000001</v>
+      </c>
       <c r="G3" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>282.62775934199999</v>
       </c>
       <c r="H3" s="10"/>
-      <c r="I3" t="e">
+      <c r="I3">
         <f>MEDIAN(E22:E33)</f>
-        <v>#NUM!</v>
+        <v>42.911500000000004</v>
       </c>
       <c r="J3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="19">
+        <v>42.803899999999999</v>
+      </c>
+      <c r="F4" s="7">
+        <v>13562.6752</v>
+      </c>
       <c r="G4" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>132.64296345599999</v>
       </c>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="19">
+        <v>42.743400000000001</v>
+      </c>
+      <c r="F5" s="7">
+        <v>19142.241000000002</v>
+      </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>187.21111698000001</v>
       </c>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="67"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71">
+      <c r="A6" s="57"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
         <v>1.25</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="19">
+        <v>43.0077</v>
+      </c>
+      <c r="F6" s="7">
+        <v>17372.050599999999</v>
+      </c>
       <c r="G6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>169.89865486799999</v>
       </c>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="19">
+        <v>43.317100000000003</v>
+      </c>
+      <c r="F7" s="7">
+        <v>17155.167000000001</v>
+      </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>167.77753325999998</v>
       </c>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="19">
+        <v>42.781999999999996</v>
+      </c>
+      <c r="F8" s="7">
+        <v>17546.924999999999</v>
+      </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>171.6089265</v>
       </c>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="19">
+        <v>42.639200000000002</v>
+      </c>
+      <c r="F9" s="7">
+        <v>21943.0537</v>
+      </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>214.60306518599998</v>
       </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71">
+      <c r="A10" s="57"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
         <v>1.25</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="19">
+        <v>43.015999999999998</v>
+      </c>
+      <c r="F10" s="7">
+        <v>14638.3084</v>
+      </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>143.16265615199998</v>
       </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="19">
+        <v>43.168100000000003</v>
+      </c>
+      <c r="F11" s="7">
+        <v>18869.616699999999</v>
+      </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>184.54485132600001</v>
       </c>
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="19">
+        <v>43.075299999999999</v>
+      </c>
+      <c r="F12" s="7">
+        <v>18976.146799999999</v>
+      </c>
       <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>185.58671570399997</v>
       </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="19">
+        <v>42.651699999999998</v>
+      </c>
+      <c r="F13" s="7">
+        <v>13453.616400000001</v>
+      </c>
       <c r="G13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>131.57636839200001</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71">
+      <c r="A14" s="57"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -2993,9 +3174,9 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -3012,9 +3193,9 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -3031,9 +3212,9 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -3050,260 +3231,324 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
-      <c r="B18" s="63">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="71"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="19">
+        <v>43.224899999999998</v>
+      </c>
+      <c r="F18" s="7">
+        <v>21085.690399999999</v>
+      </c>
       <c r="G18" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>206.21805211200001</v>
       </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="71"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="19">
+        <v>43.070399999999999</v>
+      </c>
+      <c r="F19" s="7">
+        <v>28806.365399999999</v>
+      </c>
       <c r="G19" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>281.72625361199999</v>
       </c>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="71"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="19">
+        <v>42.790599999999998</v>
+      </c>
+      <c r="F20" s="7">
+        <v>15239.090700000001</v>
+      </c>
       <c r="G20" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149.038307046</v>
       </c>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="71"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="19">
+        <v>42.600200000000001</v>
+      </c>
+      <c r="F21" s="7">
+        <v>21023.6512</v>
+      </c>
       <c r="G21" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>205.61130873600001</v>
       </c>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="71">
+      <c r="A22" s="57"/>
+      <c r="B22" s="63">
         <v>0.75</v>
       </c>
-      <c r="C22" s="71"/>
+      <c r="C22" s="63"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="43">
+        <v>43.5535</v>
+      </c>
+      <c r="F22" s="7">
+        <v>28398.577499999999</v>
+      </c>
       <c r="G22" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>277.73808795000002</v>
       </c>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="19">
+        <v>42.841500000000003</v>
+      </c>
+      <c r="F23" s="7">
+        <v>15143.5447</v>
+      </c>
       <c r="G23" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>148.10386716600001</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="19">
+        <v>42.864899999999999</v>
+      </c>
+      <c r="F24" s="7">
+        <v>15511.613799999999</v>
+      </c>
       <c r="G24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>151.70358296399999</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="19">
+        <v>42.7483</v>
+      </c>
+      <c r="F25" s="7">
+        <v>15278.832200000001</v>
+      </c>
       <c r="G25" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149.42697891600002</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="71">
+      <c r="A26" s="57"/>
+      <c r="B26" s="63">
         <v>0.5</v>
       </c>
-      <c r="C26" s="71"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="19">
+        <v>42.835700000000003</v>
+      </c>
+      <c r="F26" s="7">
+        <v>16382.6392</v>
+      </c>
       <c r="G26" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>160.22221137599999</v>
       </c>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="19">
+        <v>42.958100000000002</v>
+      </c>
+      <c r="F27" s="7">
+        <v>21066.618699999999</v>
+      </c>
       <c r="G27" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>206.03153088599998</v>
       </c>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="19">
+        <v>43.039200000000001</v>
+      </c>
+      <c r="F28" s="7">
+        <v>28106.2274</v>
+      </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>274.87890397199999</v>
       </c>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="19">
+        <v>42.669800000000002</v>
+      </c>
+      <c r="F29" s="7">
+        <v>15577.2039</v>
+      </c>
       <c r="G29" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>152.34505414200001</v>
       </c>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="67"/>
-      <c r="B30" s="71">
+      <c r="A30" s="57"/>
+      <c r="B30" s="63">
         <v>0.25</v>
       </c>
-      <c r="C30" s="71"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="19">
+        <v>43.164299999999997</v>
+      </c>
+      <c r="F30" s="7">
+        <v>20855.140200000002</v>
+      </c>
       <c r="G30" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>203.96327115599999</v>
       </c>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="19">
+        <v>43.258899999999997</v>
+      </c>
+      <c r="F31" s="7">
+        <v>28827.166700000002</v>
+      </c>
       <c r="G31" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>281.92969032600001</v>
       </c>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="19">
+        <v>42.993200000000002</v>
+      </c>
+      <c r="F32" s="7">
+        <v>15442.696900000001</v>
+      </c>
       <c r="G32" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>151.02957568200003</v>
       </c>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="68"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="9"/>
+      <c r="E33" s="21">
+        <v>42.7181</v>
+      </c>
+      <c r="F33" s="9">
+        <v>15320.4329</v>
+      </c>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149.83383376199998</v>
       </c>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="73">
+      <c r="B34" s="65">
         <v>0.1</v>
       </c>
-      <c r="C34" s="73">
+      <c r="C34" s="65">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -3322,9 +3567,9 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="49"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -3341,9 +3586,9 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="49"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -3360,9 +3605,9 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="48"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -3382,11 +3627,11 @@
       <c r="A38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="8">
         <v>43.123899999999999</v>
       </c>
@@ -3403,10 +3648,10 @@
       <c r="A39" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="87"/>
+      <c r="C39" s="96"/>
       <c r="D39" s="40" t="s">
         <v>16</v>
       </c>
@@ -3424,13 +3669,13 @@
     </row>
     <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="88"/>
-      <c r="D40" s="89"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="98"/>
       <c r="E40" s="42">
         <v>43.224200000000003</v>
       </c>
@@ -3444,12 +3689,12 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="5">
         <v>42.909700000000001</v>
       </c>
@@ -3475,13 +3720,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
@@ -3492,6 +3730,13 @@
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3501,10 +3746,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3B9CA8-3DBF-4B1E-ADDB-145C612FA0E4}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3549,19 +3794,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -3728,336 +3973,377 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="9">
         <v>43.224200000000003</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="45">
         <v>33.56</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="45">
         <v>53.02</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="45">
         <v>67.62</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="45">
         <v>0.52610000000000001</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="45">
         <v>0.73329999999999995</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="45">
         <v>1026</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="45">
         <v>0.73619999999999997</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="45">
         <v>1030</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="45">
         <v>0.73619999999999997</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="45">
         <v>1030</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="5">
         <v>43.105200000000004</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="24">
         <v>33.86</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="24">
         <v>53.03</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="24">
         <v>68.69</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="24">
         <v>0.51370000000000005</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="24">
         <v>0.74839999999999995</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="24">
         <v>1047</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="24">
         <v>0.75049999999999994</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="24">
         <v>1050</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="24">
         <v>0.75049999999999994</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="24">
         <v>1050</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="31">
-        <v>43.406100000000002</v>
-      </c>
-      <c r="D8" s="32">
-        <v>33.82</v>
-      </c>
-      <c r="E8" s="32">
-        <v>53.02</v>
-      </c>
-      <c r="F8" s="32">
-        <v>68.540000000000006</v>
-      </c>
-      <c r="G8" s="32">
-        <v>0.52449999999999997</v>
-      </c>
-      <c r="H8" s="32">
-        <v>0.74839999999999995</v>
-      </c>
-      <c r="I8" s="32">
-        <v>1047</v>
-      </c>
-      <c r="J8" s="32">
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="K8" s="32">
-        <v>1051</v>
-      </c>
-      <c r="L8" s="32">
-        <v>0.75129999999999997</v>
-      </c>
-      <c r="M8" s="32">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="34">
-        <v>43.305199999999999</v>
-      </c>
-      <c r="D9" s="28">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="E9" s="28">
-        <v>53.32</v>
-      </c>
-      <c r="F9" s="28">
-        <v>67.87</v>
-      </c>
-      <c r="G9" s="28">
-        <v>0.52629999999999999</v>
-      </c>
-      <c r="H9" s="28">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="I9" s="28">
-        <v>1050</v>
-      </c>
-      <c r="J9" s="28">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="K9" s="28">
-        <v>1054</v>
-      </c>
-      <c r="L9" s="28">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M9" s="28">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="B11" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="32">
+        <v>43.5535</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C15" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D15" s="5">
         <v>37.71</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E15" s="5">
         <v>55.04</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F15" s="5">
         <v>66.48</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G15" s="5">
         <v>0.5131</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H15" s="5">
         <v>0.76480000000000004</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I15" s="5">
         <v>1070</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J15" s="5">
         <v>0.76700000000000002</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K15" s="5">
         <v>1073</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L15" s="5">
         <v>0.76700000000000002</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M15" s="5">
         <v>1073</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="7">
+      <c r="C16" s="84"/>
+      <c r="D16" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E16" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="79"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="88"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B17" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="7">
+      <c r="C17" s="84"/>
+      <c r="D17" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="82"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="E17" s="89"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="91"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="7">
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="80"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="91"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="7">
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="E19" s="89"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="91"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="7">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="85"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="94"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="E11:M15"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="E16:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4115,19 +4401,19 @@
         <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -4135,7 +4421,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>52</v>
@@ -4381,7 +4667,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="31">
         <v>40.930199999999999</v>
@@ -4419,10 +4705,10 @@
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="34">
         <v>40.607199999999999</v>
@@ -4465,7 +4751,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="84" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
@@ -4506,99 +4792,99 @@
       <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="7">
         <v>36.130000000000003</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="79"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="88"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="7">
         <v>35.5</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="82"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="91"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="7">
         <v>35.409999999999997</v>
       </c>
-      <c r="E13" s="80"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="91"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="7">
         <v>35.18</v>
       </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="91"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="76"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="7">
         <v>31.63</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="85"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="94"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="23"/>
@@ -4621,11 +4907,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4858,27 +5145,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4903,9 +5180,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update adapt-wce trial logs
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1896" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DCB0588-3ABB-4BCF-8084-1B1613D36764}"/>
+  <xr:revisionPtr revIDLastSave="1922" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BCFBF6F-D4B3-4101-A551-66EE7521E62C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
-    <sheet name="opus_base Simple WCE" sheetId="10" r:id="rId2"/>
-    <sheet name="opus_base Fine WCE" sheetId="12" r:id="rId3"/>
-    <sheet name="opus_base AoN WCE" sheetId="13" r:id="rId4"/>
+    <sheet name="opus_base Simple aWCE" sheetId="10" r:id="rId2"/>
+    <sheet name="opus_base Fine aWCE" sheetId="12" r:id="rId3"/>
+    <sheet name="opus_base AoN aWCE" sheetId="13" r:id="rId4"/>
     <sheet name="opus_base Test" sheetId="2" r:id="rId5"/>
     <sheet name="opus_big Validation" sheetId="7" r:id="rId6"/>
-    <sheet name="opus_big Simple WCE" sheetId="11" r:id="rId7"/>
-    <sheet name="opus_big Fine WCE" sheetId="14" r:id="rId8"/>
-    <sheet name="opus_big AoN WCE" sheetId="15" r:id="rId9"/>
+    <sheet name="opus_big Simple aWCE" sheetId="11" r:id="rId7"/>
+    <sheet name="opus_big Fine aWCE" sheetId="14" r:id="rId8"/>
+    <sheet name="opus_big AoN aWCE" sheetId="15" r:id="rId9"/>
     <sheet name="opus_big Test " sheetId="4" r:id="rId10"/>
     <sheet name="M2M (Deprecated)" sheetId="6" state="hidden" r:id="rId11"/>
   </sheets>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="79">
   <si>
     <t>Weight</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>0.1 train sample, full glossary, upper weight 1.25, bands 6</t>
-  </si>
-  <si>
-    <t>RERUN</t>
   </si>
   <si>
     <t>Fine-Banded Adaptive WCE</t>
@@ -892,6 +889,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -913,12 +967,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,57 +977,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1345,7 +1342,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1386,13 +1383,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="66">
+      <c r="C2" s="85">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1414,9 +1411,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1436,9 +1433,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1458,9 +1455,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1480,9 +1477,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74">
+      <c r="A6" s="87"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1504,9 +1501,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1526,9 +1523,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1548,9 +1545,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1570,9 +1567,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74">
+      <c r="A10" s="87"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1594,9 +1591,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1616,9 +1613,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1638,9 +1635,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="68"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1660,9 +1657,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="68"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74">
+      <c r="A14" s="87"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1684,9 +1681,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="68"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1706,9 +1703,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="68"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1728,9 +1725,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1750,11 +1747,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="64">
+      <c r="A18" s="87"/>
+      <c r="B18" s="83">
         <v>1</v>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="91"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1774,9 +1771,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="68"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="74"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1796,9 +1793,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="68"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="74"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1818,9 +1815,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="68"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="74"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1840,11 +1837,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="68"/>
-      <c r="B22" s="74">
+      <c r="A22" s="87"/>
+      <c r="B22" s="91">
         <v>0.75</v>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1864,9 +1861,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="68"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1885,9 +1882,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="68"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
+      <c r="A24" s="87"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1907,9 +1904,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="68"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1929,11 +1926,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="68"/>
-      <c r="B26" s="74">
+      <c r="A26" s="87"/>
+      <c r="B26" s="91">
         <v>0.5</v>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1953,9 +1950,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="68"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1963,21 +1960,21 @@
         <v>42.8322</v>
       </c>
       <c r="F27" s="25">
-        <v>25586.411599999999</v>
+        <v>25698.797900000001</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>7.1073365555555554</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>71</v>
+        <v>7.1385549722222228</v>
+      </c>
+      <c r="H27" s="7">
+        <v>137.96010000000001</v>
       </c>
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="68"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1997,9 +1994,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -2007,23 +2004,23 @@
         <v>42.115699999999997</v>
       </c>
       <c r="F29" s="25">
-        <v>15740.974700000001</v>
+        <v>15399.811</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
-        <v>4.3724929722222221</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>71</v>
+        <v>4.2777252777777779</v>
+      </c>
+      <c r="H29" s="5">
+        <v>69.000799999999998</v>
       </c>
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="68"/>
-      <c r="B30" s="74">
+      <c r="A30" s="87"/>
+      <c r="B30" s="91">
         <v>0.25</v>
       </c>
-      <c r="C30" s="74"/>
+      <c r="C30" s="91"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -2043,9 +2040,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="68"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -2065,9 +2062,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="68"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -2087,9 +2084,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="92"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -2109,13 +2106,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="70" t="s">
+      <c r="A34" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="76">
+      <c r="B34" s="93">
         <v>0.1</v>
       </c>
-      <c r="C34" s="76">
+      <c r="C34" s="93">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -2137,9 +2134,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="71"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="74"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="91"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -2159,9 +2156,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="91"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -2181,9 +2178,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="72"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="92"/>
+      <c r="C37" s="92"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -2203,14 +2200,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="85"/>
-      <c r="D38" s="86"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -2227,12 +2224,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="72"/>
-      <c r="B39" s="78" t="s">
+      <c r="A39" s="68"/>
+      <c r="B39" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="80"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="14">
         <v>42.128999999999998</v>
       </c>
@@ -2249,13 +2246,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="92"/>
+      <c r="C40" s="81"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -2277,9 +2274,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="71"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="93"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="82"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -2301,11 +2298,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="71"/>
-      <c r="B42" s="87" t="s">
+      <c r="A42" s="69"/>
+      <c r="B42" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="88"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -2327,9 +2324,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="72"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -2351,14 +2348,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="81" t="s">
+      <c r="B44" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="82"/>
-      <c r="D44" s="83"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="66"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -2375,12 +2372,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="72"/>
-      <c r="B45" s="78" t="s">
+      <c r="A45" s="68"/>
+      <c r="B45" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="79"/>
-      <c r="D45" s="80"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="72"/>
       <c r="E45" s="14">
         <v>42.606000000000002</v>
       </c>
@@ -2397,12 +2394,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="73" t="s">
+      <c r="A46" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2429,13 +2426,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2452,6 +2442,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2464,7 +2461,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,7 +2774,9 @@
       <c r="B8" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="25">
+        <v>43.083300000000001</v>
+      </c>
       <c r="D8" s="24">
         <v>33.47</v>
       </c>
@@ -2814,7 +2813,9 @@
         <v>61</v>
       </c>
       <c r="B9" s="95"/>
-      <c r="C9" s="25"/>
+      <c r="C9" s="25">
+        <v>43.3155</v>
+      </c>
       <c r="D9" s="24">
         <v>33.86</v>
       </c>
@@ -2851,7 +2852,9 @@
         <v>58</v>
       </c>
       <c r="B10" s="108"/>
-      <c r="C10" s="26"/>
+      <c r="C10" s="26">
+        <v>43.175699999999999</v>
+      </c>
       <c r="D10" s="32">
         <v>33.409999999999997</v>
       </c>
@@ -2931,7 +2934,9 @@
       <c r="B12" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="46">
+        <v>42.999899999999997</v>
+      </c>
       <c r="D12" s="46">
         <v>34.82</v>
       </c>
@@ -2968,7 +2973,9 @@
         <v>62</v>
       </c>
       <c r="B13" s="117"/>
-      <c r="C13" s="46"/>
+      <c r="C13" s="46">
+        <v>42.972000000000001</v>
+      </c>
       <c r="D13" s="46">
         <v>34.590000000000003</v>
       </c>
@@ -3005,7 +3012,9 @@
         <v>60</v>
       </c>
       <c r="B14" s="118"/>
-      <c r="C14" s="47"/>
+      <c r="C14" s="47">
+        <v>43.414900000000003</v>
+      </c>
       <c r="D14" s="47">
         <v>34.200000000000003</v>
       </c>
@@ -3039,7 +3048,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="57"/>
       <c r="C15" s="31"/>
@@ -3056,7 +3065,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="55"/>
       <c r="C16" s="46"/>
@@ -3073,7 +3082,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="47"/>
@@ -3822,7 +3831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C20E6-94C4-4B99-8775-24B7DED1396E}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -3838,10 +3847,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -4080,8 +4089,8 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="98">
         <v>4</v>
@@ -4097,7 +4106,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -4110,7 +4119,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -4123,7 +4132,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -4136,7 +4145,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="98">
         <v>5</v>
       </c>
@@ -4151,7 +4160,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -4163,7 +4172,7 @@
       <c r="H23" s="61"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -4176,7 +4185,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -4189,7 +4198,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="98">
         <v>6</v>
       </c>
@@ -4204,7 +4213,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -4217,7 +4226,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -4230,7 +4239,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -4243,7 +4252,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="98">
         <v>7</v>
       </c>
@@ -4258,7 +4267,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -4271,7 +4280,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -4284,7 +4293,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -4487,10 +4496,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -4695,8 +4704,8 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="98">
         <v>0</v>
@@ -4710,7 +4719,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -4721,7 +4730,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -4732,7 +4741,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -4743,7 +4752,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="98">
         <v>1</v>
       </c>
@@ -4756,7 +4765,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -4767,7 +4776,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -4778,7 +4787,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -4789,7 +4798,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="98">
         <v>2</v>
       </c>
@@ -4802,7 +4811,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -4813,7 +4822,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -4824,7 +4833,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -4835,7 +4844,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="98">
         <v>3</v>
       </c>
@@ -4848,7 +4857,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -4859,7 +4868,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -4870,7 +4879,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -4884,16 +4893,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4921,10 +4930,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -5129,8 +5138,8 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="94">
         <v>0.2</v>
@@ -5144,7 +5153,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="95"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -5155,7 +5164,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="95"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -5166,7 +5175,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="96"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -5177,7 +5186,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="97">
         <v>0.4</v>
       </c>
@@ -5190,7 +5199,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="95"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -5201,7 +5210,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="95"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -5212,7 +5221,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="96"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -5223,7 +5232,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="97">
         <v>0.6</v>
       </c>
@@ -5236,7 +5245,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="95"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -5247,7 +5256,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="95"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -5258,7 +5267,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="96"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -5269,7 +5278,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="97">
         <v>0.8</v>
       </c>
@@ -5282,7 +5291,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="95"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -5293,7 +5302,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="95"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -5304,7 +5313,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="96"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -5316,16 +5325,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5337,8 +5346,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5651,7 +5660,9 @@
       <c r="B8" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18">
+        <v>42.563800000000001</v>
+      </c>
       <c r="D8" s="24">
         <v>33.96</v>
       </c>
@@ -5688,7 +5699,9 @@
         <v>61</v>
       </c>
       <c r="B9" s="95"/>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18">
+        <v>42.523899999999998</v>
+      </c>
       <c r="D9" s="24">
         <v>33.369999999999997</v>
       </c>
@@ -5725,7 +5738,9 @@
         <v>58</v>
       </c>
       <c r="B10" s="108"/>
-      <c r="C10" s="20"/>
+      <c r="C10" s="20">
+        <v>42.845599999999997</v>
+      </c>
       <c r="D10" s="32">
         <v>33.26</v>
       </c>
@@ -5805,7 +5820,9 @@
       <c r="B12" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="50"/>
+      <c r="C12" s="50">
+        <v>42.973199999999999</v>
+      </c>
       <c r="D12" s="49">
         <v>33.39</v>
       </c>
@@ -5842,7 +5859,9 @@
         <v>62</v>
       </c>
       <c r="B13" s="110"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="50">
+        <v>42.744900000000001</v>
+      </c>
       <c r="D13" s="49">
         <v>33.46</v>
       </c>
@@ -5879,7 +5898,9 @@
         <v>60</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="29"/>
+      <c r="C14" s="29">
+        <v>42.728999999999999</v>
+      </c>
       <c r="D14" s="28">
         <v>33.450000000000003</v>
       </c>
@@ -5913,7 +5934,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="54"/>
@@ -5930,7 +5951,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -5947,7 +5968,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -6168,13 +6189,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="66">
+      <c r="C2" s="85">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -6196,9 +6217,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -6218,9 +6239,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -6240,9 +6261,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -6262,9 +6283,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74">
+      <c r="A6" s="87"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -6286,9 +6307,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -6308,9 +6329,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -6330,9 +6351,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -6352,9 +6373,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74">
+      <c r="A10" s="87"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -6376,9 +6397,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -6398,9 +6419,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -6420,9 +6441,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="68"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -6442,9 +6463,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="68"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74">
+      <c r="A14" s="87"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -6466,9 +6487,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="68"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -6488,9 +6509,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="68"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -6510,9 +6531,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -6532,11 +6553,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="64">
+      <c r="A18" s="87"/>
+      <c r="B18" s="83">
         <v>1</v>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="91"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -6556,9 +6577,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="68"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="74"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -6578,9 +6599,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="68"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="74"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -6600,9 +6621,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="68"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="74"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -6622,11 +6643,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="68"/>
-      <c r="B22" s="74">
+      <c r="A22" s="87"/>
+      <c r="B22" s="91">
         <v>0.75</v>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -6646,9 +6667,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="68"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -6667,9 +6688,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="68"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
+      <c r="A24" s="87"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -6689,9 +6710,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="68"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -6711,11 +6732,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="68"/>
-      <c r="B26" s="74">
+      <c r="A26" s="87"/>
+      <c r="B26" s="91">
         <v>0.5</v>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -6735,9 +6756,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="68"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -6757,9 +6778,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="68"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -6779,9 +6800,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -6801,11 +6822,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="68"/>
-      <c r="B30" s="74">
+      <c r="A30" s="87"/>
+      <c r="B30" s="91">
         <v>0.25</v>
       </c>
-      <c r="C30" s="74"/>
+      <c r="C30" s="91"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -6825,9 +6846,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="68"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -6847,9 +6868,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="68"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -6869,9 +6890,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="92"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -6891,13 +6912,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="70" t="s">
+      <c r="A34" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="76">
+      <c r="B34" s="93">
         <v>0.1</v>
       </c>
-      <c r="C34" s="76">
+      <c r="C34" s="93">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -6919,9 +6940,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="71"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="74"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="91"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -6941,9 +6962,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="91"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -6963,9 +6984,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="72"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="92"/>
+      <c r="C37" s="92"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -6988,11 +7009,11 @@
       <c r="A38" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="78" t="s">
+      <c r="B38" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="79"/>
-      <c r="D38" s="80"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="8">
         <v>43.123899999999999</v>
       </c>
@@ -7040,7 +7061,7 @@
       <c r="A40" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="89" t="s">
+      <c r="B40" s="78" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="114"/>
@@ -7061,12 +7082,12 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
+      <c r="A41" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
       <c r="E41" s="5">
         <v>42.909700000000001</v>
       </c>
@@ -7093,6 +7114,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
@@ -7103,13 +7131,6 @@
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7137,10 +7158,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -7345,8 +7366,8 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="98">
         <v>4</v>
@@ -7360,7 +7381,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -7371,7 +7392,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -7382,7 +7403,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -7393,7 +7414,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="98">
         <v>5</v>
       </c>
@@ -7406,7 +7427,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -7417,7 +7438,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -7428,7 +7449,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -7439,7 +7460,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="98">
         <v>6</v>
       </c>
@@ -7452,7 +7473,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -7463,7 +7484,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -7474,7 +7495,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -7485,7 +7506,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="98">
         <v>7</v>
       </c>
@@ -7498,7 +7519,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -7509,7 +7530,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -7520,7 +7541,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -7532,16 +7553,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7553,7 +7574,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7569,10 +7590,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -7777,8 +7798,8 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="98">
         <v>0</v>
@@ -7792,7 +7813,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -7803,7 +7824,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -7814,7 +7835,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -7825,7 +7846,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="98">
         <v>1</v>
       </c>
@@ -7838,7 +7859,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -7849,7 +7870,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -7860,7 +7881,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -7871,7 +7892,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="98">
         <v>2</v>
       </c>
@@ -7884,7 +7905,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -7895,7 +7916,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -7906,7 +7927,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -7917,7 +7938,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="98">
         <v>3</v>
       </c>
@@ -7930,7 +7951,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -7941,7 +7962,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -7952,7 +7973,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -7964,16 +7985,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8001,10 +8022,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -8209,8 +8230,8 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>77</v>
+      <c r="A18" s="83" t="s">
+        <v>76</v>
       </c>
       <c r="B18" s="95">
         <v>0.2</v>
@@ -8224,7 +8245,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="95"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -8235,7 +8256,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="95"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -8246,7 +8267,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="96"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -8257,7 +8278,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="97">
         <v>0.4</v>
       </c>
@@ -8270,7 +8291,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="95"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -8281,7 +8302,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="95"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -8292,7 +8313,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="96"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -8303,7 +8324,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="97">
         <v>0.6</v>
       </c>
@@ -8316,7 +8337,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="95"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -8327,7 +8348,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="95"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -8338,7 +8359,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="96"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -8349,7 +8370,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="84"/>
       <c r="B30" s="97">
         <v>0.8</v>
       </c>
@@ -8362,7 +8383,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="95"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -8373,7 +8394,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="95"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -8384,7 +8405,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="96"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -8397,16 +8418,16 @@
     <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8414,12 +8435,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8652,17 +8672,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8687,18 +8717,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update model predictions and results
</commit_message>
<xml_diff>
--- a/model_evaluations/Collated Validation and Test Set Results.xlsx
+++ b/model_evaluations/Collated Validation and Test Set Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1922" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BCFBF6F-D4B3-4101-A551-66EE7521E62C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -889,6 +889,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -898,24 +949,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -944,39 +977,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1342,7 +1342,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B18" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,13 +1383,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="66">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1411,9 +1411,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="87"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1433,9 +1433,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1455,9 +1455,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="87"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1477,9 +1477,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="87"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91">
+      <c r="A6" s="68"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1501,9 +1501,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="87"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1523,9 +1523,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1545,9 +1545,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="87"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1567,9 +1567,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="87"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91">
+      <c r="A10" s="68"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1591,9 +1591,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="87"/>
-      <c r="B11" s="91"/>
-      <c r="C11" s="91"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1613,9 +1613,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="87"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1635,9 +1635,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="87"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1657,9 +1657,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="87"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91">
+      <c r="A14" s="68"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1681,9 +1681,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="87"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1703,9 +1703,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="87"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1725,9 +1725,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="87"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1747,11 +1747,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="87"/>
-      <c r="B18" s="83">
+      <c r="A18" s="68"/>
+      <c r="B18" s="64">
         <v>1</v>
       </c>
-      <c r="C18" s="91"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1771,9 +1771,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="87"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="91"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1793,9 +1793,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="87"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1815,9 +1815,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="87"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1837,11 +1837,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="87"/>
-      <c r="B22" s="91">
+      <c r="A22" s="68"/>
+      <c r="B22" s="74">
         <v>0.75</v>
       </c>
-      <c r="C22" s="91"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1861,9 +1861,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="87"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1882,9 +1882,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="87"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1904,9 +1904,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="87"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1926,11 +1926,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="87"/>
-      <c r="B26" s="91">
+      <c r="A26" s="68"/>
+      <c r="B26" s="74">
         <v>0.5</v>
       </c>
-      <c r="C26" s="91"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1950,9 +1950,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1972,9 +1972,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="87"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1994,9 +1994,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="87"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -2016,11 +2016,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="87"/>
-      <c r="B30" s="91">
+      <c r="A30" s="68"/>
+      <c r="B30" s="74">
         <v>0.25</v>
       </c>
-      <c r="C30" s="91"/>
+      <c r="C30" s="74"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -2040,9 +2040,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="87"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -2062,9 +2062,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="87"/>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -2084,9 +2084,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="88"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="92"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -2106,13 +2106,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="89" t="s">
+      <c r="A34" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="93">
+      <c r="B34" s="76">
         <v>0.1</v>
       </c>
-      <c r="C34" s="93">
+      <c r="C34" s="76">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -2134,9 +2134,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="74"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -2156,9 +2156,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="69"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -2178,9 +2178,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="68"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -2200,14 +2200,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="75"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="86"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -2224,12 +2224,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="68"/>
-      <c r="B39" s="70" t="s">
+      <c r="A39" s="72"/>
+      <c r="B39" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="72"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="14">
         <v>42.128999999999998</v>
       </c>
@@ -2246,13 +2246,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="81"/>
+      <c r="C40" s="92"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -2274,9 +2274,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="69"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="82"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -2298,11 +2298,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="69"/>
-      <c r="B42" s="76" t="s">
+      <c r="A42" s="71"/>
+      <c r="B42" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="88"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -2324,9 +2324,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="68"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="79"/>
+      <c r="A43" s="72"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="90"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -2348,14 +2348,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="65"/>
-      <c r="D44" s="66"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="83"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -2372,12 +2372,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="68"/>
-      <c r="B45" s="70" t="s">
+      <c r="A45" s="72"/>
+      <c r="B45" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="80"/>
       <c r="E45" s="14">
         <v>42.606000000000002</v>
       </c>
@@ -2394,12 +2394,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="90"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2426,6 +2426,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2442,13 +2449,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2461,7 +2461,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4089,7 +4089,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="98">
@@ -4106,7 +4106,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -4119,7 +4119,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -4132,7 +4132,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -4145,7 +4145,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="98">
         <v>5</v>
       </c>
@@ -4160,7 +4160,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -4172,7 +4172,7 @@
       <c r="H23" s="61"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -4185,7 +4185,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -4198,7 +4198,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="98">
         <v>6</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -4226,7 +4226,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -4239,7 +4239,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -4252,7 +4252,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="98">
         <v>7</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -4280,7 +4280,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -4293,7 +4293,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -4704,7 +4704,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="98">
@@ -4719,7 +4719,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -4730,7 +4730,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -4741,7 +4741,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -4752,7 +4752,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="98">
         <v>1</v>
       </c>
@@ -4765,7 +4765,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -4776,7 +4776,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -4787,7 +4787,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -4798,7 +4798,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="98">
         <v>2</v>
       </c>
@@ -4811,7 +4811,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -4822,7 +4822,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -4833,7 +4833,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -4844,7 +4844,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="98">
         <v>3</v>
       </c>
@@ -4857,7 +4857,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -4868,7 +4868,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -4879,7 +4879,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -4893,16 +4893,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5138,7 +5138,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="94">
@@ -5153,7 +5153,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="95"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -5164,7 +5164,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="95"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -5175,7 +5175,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="96"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -5186,7 +5186,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="97">
         <v>0.4</v>
       </c>
@@ -5199,7 +5199,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="95"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -5210,7 +5210,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="95"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -5221,7 +5221,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="96"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -5232,7 +5232,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="97">
         <v>0.6</v>
       </c>
@@ -5245,7 +5245,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="95"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -5256,7 +5256,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="95"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -5267,7 +5267,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="96"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -5278,7 +5278,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="97">
         <v>0.8</v>
       </c>
@@ -5291,7 +5291,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="95"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -5302,7 +5302,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="95"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -5313,7 +5313,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="96"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -5325,16 +5325,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5347,7 +5347,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6147,7 +6147,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -6189,13 +6189,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="66">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -6217,9 +6217,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="87"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -6239,9 +6239,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -6261,9 +6261,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="87"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -6283,9 +6283,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="87"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91">
+      <c r="A6" s="68"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -6307,9 +6307,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="87"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -6329,9 +6329,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -6351,9 +6351,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="87"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -6373,9 +6373,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="87"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91">
+      <c r="A10" s="68"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -6397,9 +6397,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="87"/>
-      <c r="B11" s="91"/>
-      <c r="C11" s="91"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -6419,9 +6419,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="87"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -6441,9 +6441,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="87"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -6463,9 +6463,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="87"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91">
+      <c r="A14" s="68"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -6487,9 +6487,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="87"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -6509,9 +6509,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="87"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -6531,9 +6531,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="87"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -6553,11 +6553,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="87"/>
-      <c r="B18" s="83">
+      <c r="A18" s="68"/>
+      <c r="B18" s="64">
         <v>1</v>
       </c>
-      <c r="C18" s="91"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -6577,9 +6577,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="87"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="91"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -6599,9 +6599,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="87"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -6621,9 +6621,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="87"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -6643,11 +6643,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="87"/>
-      <c r="B22" s="91">
+      <c r="A22" s="68"/>
+      <c r="B22" s="74">
         <v>0.75</v>
       </c>
-      <c r="C22" s="91"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -6667,9 +6667,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="87"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -6688,9 +6688,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="87"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -6710,9 +6710,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="87"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -6732,11 +6732,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="87"/>
-      <c r="B26" s="91">
+      <c r="A26" s="68"/>
+      <c r="B26" s="74">
         <v>0.5</v>
       </c>
-      <c r="C26" s="91"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -6756,9 +6756,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -6778,9 +6778,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="87"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -6800,9 +6800,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="87"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -6822,11 +6822,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="87"/>
-      <c r="B30" s="91">
+      <c r="A30" s="68"/>
+      <c r="B30" s="74">
         <v>0.25</v>
       </c>
-      <c r="C30" s="91"/>
+      <c r="C30" s="74"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -6846,9 +6846,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="87"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -6868,9 +6868,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="87"/>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -6890,9 +6890,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="88"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="92"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -6912,13 +6912,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="89" t="s">
+      <c r="A34" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="93">
+      <c r="B34" s="76">
         <v>0.1</v>
       </c>
-      <c r="C34" s="93">
+      <c r="C34" s="76">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -6940,9 +6940,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="74"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -6962,9 +6962,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="69"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -6984,9 +6984,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="68"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -7009,11 +7009,11 @@
       <c r="A38" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="72"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
       <c r="E38" s="8">
         <v>43.123899999999999</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="A40" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="114"/>
@@ -7082,12 +7082,12 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="5">
         <v>42.909700000000001</v>
       </c>
@@ -7114,13 +7114,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
@@ -7131,6 +7124,13 @@
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7366,7 +7366,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="98">
@@ -7381,7 +7381,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -7392,7 +7392,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -7403,7 +7403,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -7414,7 +7414,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="98">
         <v>5</v>
       </c>
@@ -7427,7 +7427,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -7438,7 +7438,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -7449,7 +7449,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -7460,7 +7460,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="98">
         <v>6</v>
       </c>
@@ -7473,7 +7473,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -7484,7 +7484,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -7495,7 +7495,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -7506,7 +7506,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="98">
         <v>7</v>
       </c>
@@ -7519,7 +7519,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -7530,7 +7530,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -7541,7 +7541,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -7553,16 +7553,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7798,7 +7798,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="98">
@@ -7813,7 +7813,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="98"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -7824,7 +7824,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="98"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -7835,7 +7835,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="98"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -7846,7 +7846,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="98">
         <v>1</v>
       </c>
@@ -7859,7 +7859,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="98"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -7870,7 +7870,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="98"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -7881,7 +7881,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="98"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -7892,7 +7892,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="98">
         <v>2</v>
       </c>
@@ -7905,7 +7905,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="98"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -7916,7 +7916,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="98"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -7927,7 +7927,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="98"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -7938,7 +7938,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="98">
         <v>3</v>
       </c>
@@ -7951,7 +7951,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="98"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -7962,7 +7962,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="98"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -7973,7 +7973,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="98"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -7985,16 +7985,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8230,7 +8230,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="95">
@@ -8245,7 +8245,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="95"/>
       <c r="C19" s="43">
         <v>1.5</v>
@@ -8256,7 +8256,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="95"/>
       <c r="C20" s="43">
         <v>1.75</v>
@@ -8267,7 +8267,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="96"/>
       <c r="C21" s="43">
         <v>2</v>
@@ -8278,7 +8278,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="97">
         <v>0.4</v>
       </c>
@@ -8291,7 +8291,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="95"/>
       <c r="C23" s="43">
         <v>1.5</v>
@@ -8302,7 +8302,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="95"/>
       <c r="C24" s="43">
         <v>1.75</v>
@@ -8313,7 +8313,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="96"/>
       <c r="C25" s="43">
         <v>2</v>
@@ -8324,7 +8324,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="97">
         <v>0.6</v>
       </c>
@@ -8337,7 +8337,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="95"/>
       <c r="C27" s="43">
         <v>1.5</v>
@@ -8348,7 +8348,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="95"/>
       <c r="C28" s="43">
         <v>1.75</v>
@@ -8359,7 +8359,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="96"/>
       <c r="C29" s="43">
         <v>2</v>
@@ -8370,7 +8370,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="97">
         <v>0.8</v>
       </c>
@@ -8383,7 +8383,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="95"/>
       <c r="C31" s="43">
         <v>1.5</v>
@@ -8394,7 +8394,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="84"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="95"/>
       <c r="C32" s="43">
         <v>1.75</v>
@@ -8405,7 +8405,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="96"/>
       <c r="C33" s="43">
         <v>2</v>
@@ -8418,16 +8418,16 @@
     <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8435,11 +8435,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8672,27 +8673,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8717,9 +8708,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>